<commit_message>
Auto-committed on 2022/04/06 週三
</commit_message>
<xml_diff>
--- a/Program/Other/LM052_底稿_放款資產分類-會計部備呆計提.xlsx
+++ b/Program/Other/LM052_底稿_放款資產分類-會計部備呆計提.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="1692" windowWidth="5976" windowHeight="4428" tabRatio="901"/>
+    <workbookView xWindow="-10" yWindow="1690" windowWidth="5980" windowHeight="4430" tabRatio="901"/>
   </bookViews>
   <sheets>
     <sheet name="備呆總表" sheetId="58" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Database" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Database" localSheetId="2">#REF!</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">備呆總表!$A$1:$N$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">備呆總表!$A$1:$N$32</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'備呆總表 (2)'!$A$1:$N$31</definedName>
     <definedName name="新" localSheetId="2">#REF!</definedName>
     <definedName name="新">#REF!</definedName>
@@ -49,7 +49,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0">
+    <comment ref="U13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="14"/>
+            <color indexed="81"/>
+            <rFont val="新細明體"/>
+            <family val="1"/>
+            <charset val="136"/>
+          </rPr>
+          <t>驗算格</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0" shapeId="0">
+    <comment ref="D17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0">
+    <comment ref="F17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0" shapeId="0">
+    <comment ref="G17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -109,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0" shapeId="0">
+    <comment ref="H17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -228,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="93">
   <si>
     <t>小計</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1039,15 +1053,41 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>經辦</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>百萬元，較最高『IFRS9預期損失金額</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>百萬元』相比，提列金額尚足。</t>
+  </si>
+  <si>
+    <t>催收款折溢價與費用</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>擔保放款折溢價</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>一、依放款資產評估辦法三項標準評估後，以五類資產評估 (Ａ)金額 1,029.31 百萬元為高。
+二、依金管會104年07月24日金管保財字第10402506096號令備抵損失提存比率為放款餘額
+    1.5%評估金額為 727.81 百萬元。
+三、IFRS 9預期損失金額依據放款各相關權責單位：PD違約機率（放款審查課）、LGD違
+    約損失率（放款管理課）、EAD曝險額（放款服務課）提供相關數據，並由放款服務課
+    於預期損失計算系統完成核帳後，計算所得之預期損失金額為1,497.23百萬元。
+四、公司備抵損失至108 年03月實際提列 1,523.99 百萬元，較最高『IFRS9預期
+        損失金額』相比，提列金額尚足。
+五、陳核。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+課主管：</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+部室主管：</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3632,7 +3672,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="304">
+  <cellXfs count="305">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4172,15 +4212,33 @@
     <xf numFmtId="176" fontId="71" fillId="0" borderId="35" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="21" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="33" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="21" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="48" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="34" fillId="0" borderId="0" xfId="93" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="21" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="48" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4391,18 +4449,6 @@
     <xf numFmtId="177" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="21" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="33" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="26" fillId="0" borderId="31" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4516,9 +4562,6 @@
     </xf>
     <xf numFmtId="179" fontId="4" fillId="0" borderId="55" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="15" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5084,35 +5127,35 @@
     <tabColor indexed="13"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V49"/>
+  <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:H11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.33203125" defaultRowHeight="31.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="13.36328125" defaultRowHeight="31.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="27.44140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="3.44140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="20.77734375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.90625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="25.6328125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="3.08984375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="30.08984375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27.453125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="27.453125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="3.453125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="20.81640625" style="4" customWidth="1"/>
     <col min="12" max="12" width="24" style="4" customWidth="1"/>
-    <col min="13" max="13" width="27.109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="6.44140625" style="10" customWidth="1"/>
-    <col min="15" max="15" width="24.21875" style="10" customWidth="1"/>
-    <col min="16" max="16" width="10.21875" style="10" customWidth="1"/>
-    <col min="17" max="17" width="20.44140625" style="37" customWidth="1"/>
-    <col min="18" max="18" width="8.77734375" style="37" customWidth="1"/>
+    <col min="13" max="13" width="27.08984375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="6.453125" style="10" customWidth="1"/>
+    <col min="15" max="15" width="24.1796875" style="10" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" style="10" customWidth="1"/>
+    <col min="17" max="17" width="20.453125" style="37" customWidth="1"/>
+    <col min="18" max="18" width="8.81640625" style="37" customWidth="1"/>
     <col min="19" max="19" width="21" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" style="10" customWidth="1"/>
-    <col min="21" max="16384" width="13.33203125" style="10"/>
+    <col min="20" max="20" width="19.36328125" style="10" customWidth="1"/>
+    <col min="21" max="16384" width="13.36328125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="39.75" customHeight="1" thickBot="1">
@@ -5139,53 +5182,53 @@
       <c r="Q1" s="36"/>
       <c r="R1" s="36"/>
     </row>
-    <row r="2" spans="1:22" s="26" customFormat="1" ht="23.1" customHeight="1" thickTop="1">
-      <c r="A2" s="203" t="s">
+    <row r="2" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1" thickTop="1">
+      <c r="A2" s="209" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="204"/>
-      <c r="C2" s="207" t="s">
+      <c r="B2" s="210"/>
+      <c r="C2" s="213" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="209" t="s">
+      <c r="D2" s="215" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="204"/>
-      <c r="F2" s="227" t="s">
+      <c r="E2" s="210"/>
+      <c r="F2" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="229" t="s">
+      <c r="G2" s="235" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="230"/>
-      <c r="I2" s="239" t="s">
+      <c r="H2" s="236"/>
+      <c r="I2" s="245" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="240"/>
-      <c r="K2" s="240"/>
-      <c r="L2" s="240"/>
-      <c r="M2" s="241"/>
+      <c r="J2" s="246"/>
+      <c r="K2" s="246"/>
+      <c r="L2" s="246"/>
+      <c r="M2" s="247"/>
       <c r="N2" s="12"/>
       <c r="O2" s="112"/>
       <c r="P2" s="36"/>
       <c r="Q2" s="38"/>
     </row>
-    <row r="3" spans="1:22" s="26" customFormat="1" ht="23.1" customHeight="1">
-      <c r="A3" s="205"/>
-      <c r="B3" s="206"/>
-      <c r="C3" s="208"/>
-      <c r="D3" s="210"/>
-      <c r="E3" s="206"/>
-      <c r="F3" s="228"/>
-      <c r="G3" s="231"/>
-      <c r="H3" s="232"/>
+    <row r="3" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1">
+      <c r="A3" s="211"/>
+      <c r="B3" s="212"/>
+      <c r="C3" s="214"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="212"/>
+      <c r="F3" s="234"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="238"/>
       <c r="I3" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="235" t="s">
+      <c r="J3" s="241" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="236"/>
+      <c r="K3" s="242"/>
       <c r="L3" s="104" t="s">
         <v>73</v>
       </c>
@@ -5198,31 +5241,31 @@
       <c r="Q3" s="58"/>
     </row>
     <row r="4" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A4" s="282" t="s">
+      <c r="A4" s="284" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="284" t="s">
+      <c r="B4" s="286" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="113"/>
-      <c r="D4" s="201"/>
-      <c r="E4" s="202"/>
+      <c r="D4" s="207"/>
+      <c r="E4" s="208"/>
       <c r="F4" s="114">
         <f>SUM(C4:E4)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="211" t="s">
+      <c r="G4" s="217" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="212"/>
+      <c r="H4" s="218"/>
       <c r="I4" s="115">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J4" s="182">
+      <c r="J4" s="186">
         <f>C4*I4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="183"/>
+      <c r="K4" s="187"/>
       <c r="L4" s="116">
         <f>D4*I4</f>
         <v>0</v>
@@ -5239,27 +5282,27 @@
       <c r="T4" s="69"/>
     </row>
     <row r="5" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A5" s="283"/>
-      <c r="B5" s="285"/>
+      <c r="A5" s="285"/>
+      <c r="B5" s="287"/>
       <c r="C5" s="113"/>
-      <c r="D5" s="215"/>
-      <c r="E5" s="216"/>
+      <c r="D5" s="221"/>
+      <c r="E5" s="222"/>
       <c r="F5" s="114">
         <f t="shared" ref="F5:F11" si="0">SUM(C5:E5)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="212" t="s">
+      <c r="G5" s="218" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="286"/>
+      <c r="H5" s="288"/>
       <c r="I5" s="115">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J5" s="182">
+      <c r="J5" s="186">
         <f t="shared" ref="J5:J9" si="1">C5*I5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="183"/>
+      <c r="K5" s="187"/>
       <c r="L5" s="116">
         <f t="shared" ref="L5:L11" si="2">D5*I5</f>
         <v>0</v>
@@ -5276,31 +5319,31 @@
       <c r="T5" s="69"/>
     </row>
     <row r="6" spans="1:22" ht="46.5" customHeight="1">
-      <c r="A6" s="213" t="s">
+      <c r="A6" s="219" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="184" t="s">
+      <c r="B6" s="190" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="113"/>
-      <c r="D6" s="201"/>
-      <c r="E6" s="202"/>
+      <c r="D6" s="207"/>
+      <c r="E6" s="208"/>
       <c r="F6" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="196" t="s">
+      <c r="G6" s="202" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="214"/>
+      <c r="H6" s="220"/>
       <c r="I6" s="115">
         <v>0.02</v>
       </c>
-      <c r="J6" s="182">
+      <c r="J6" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K6" s="183"/>
+      <c r="K6" s="187"/>
       <c r="L6" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -5317,27 +5360,27 @@
       <c r="T6" s="69"/>
     </row>
     <row r="7" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A7" s="213"/>
-      <c r="B7" s="184"/>
+      <c r="A7" s="219"/>
+      <c r="B7" s="190"/>
       <c r="C7" s="121"/>
-      <c r="D7" s="242"/>
-      <c r="E7" s="243"/>
+      <c r="D7" s="248"/>
+      <c r="E7" s="249"/>
       <c r="F7" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="195" t="s">
+      <c r="G7" s="201" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="196"/>
+      <c r="H7" s="202"/>
       <c r="I7" s="115">
         <v>0.02</v>
       </c>
-      <c r="J7" s="182">
+      <c r="J7" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7" s="183"/>
+      <c r="K7" s="187"/>
       <c r="L7" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -5354,27 +5397,27 @@
       <c r="T7" s="69"/>
     </row>
     <row r="8" spans="1:22" ht="39.75" customHeight="1">
-      <c r="A8" s="213"/>
-      <c r="B8" s="184"/>
+      <c r="A8" s="219"/>
+      <c r="B8" s="190"/>
       <c r="C8" s="113"/>
-      <c r="D8" s="201"/>
-      <c r="E8" s="202"/>
+      <c r="D8" s="207"/>
+      <c r="E8" s="208"/>
       <c r="F8" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="193" t="s">
+      <c r="G8" s="199" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="194"/>
+      <c r="H8" s="200"/>
       <c r="I8" s="115">
         <v>0.02</v>
       </c>
-      <c r="J8" s="182">
+      <c r="J8" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="183"/>
+      <c r="K8" s="187"/>
       <c r="L8" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -5398,24 +5441,24 @@
         <v>22</v>
       </c>
       <c r="C9" s="113"/>
-      <c r="D9" s="191"/>
-      <c r="E9" s="192"/>
+      <c r="D9" s="197"/>
+      <c r="E9" s="198"/>
       <c r="F9" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="193" t="s">
+      <c r="G9" s="199" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="194"/>
+      <c r="H9" s="200"/>
       <c r="I9" s="122">
         <v>0.1</v>
       </c>
-      <c r="J9" s="182">
+      <c r="J9" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K9" s="183"/>
+      <c r="K9" s="187"/>
       <c r="L9" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -5439,24 +5482,24 @@
         <v>8</v>
       </c>
       <c r="C10" s="124"/>
-      <c r="D10" s="191"/>
-      <c r="E10" s="192"/>
+      <c r="D10" s="197"/>
+      <c r="E10" s="198"/>
       <c r="F10" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="193" t="s">
+      <c r="G10" s="199" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="194"/>
+      <c r="H10" s="200"/>
       <c r="I10" s="122">
         <v>0.5</v>
       </c>
-      <c r="J10" s="182">
+      <c r="J10" s="186">
         <f>C10*I10</f>
         <v>0</v>
       </c>
-      <c r="K10" s="183"/>
+      <c r="K10" s="187"/>
       <c r="L10" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -5479,24 +5522,24 @@
         <v>3</v>
       </c>
       <c r="C11" s="113"/>
-      <c r="D11" s="244"/>
-      <c r="E11" s="245"/>
+      <c r="D11" s="250"/>
+      <c r="E11" s="251"/>
       <c r="F11" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="193" t="s">
+      <c r="G11" s="199" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="194"/>
+      <c r="H11" s="200"/>
       <c r="I11" s="125">
         <v>1</v>
       </c>
-      <c r="J11" s="182">
+      <c r="J11" s="186">
         <f t="shared" ref="J11" si="4">C11*I11</f>
         <v>0</v>
       </c>
-      <c r="K11" s="183"/>
+      <c r="K11" s="187"/>
       <c r="L11" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -5512,21 +5555,23 @@
       <c r="R11" s="11"/>
     </row>
     <row r="12" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A12" s="296" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="255"/>
+      <c r="A12" s="181" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="182"/>
       <c r="C12" s="113"/>
-      <c r="D12" s="254"/>
-      <c r="E12" s="255"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="256"/>
-      <c r="H12" s="257"/>
+      <c r="D12" s="183"/>
+      <c r="E12" s="182"/>
+      <c r="F12" s="126">
+        <v>0</v>
+      </c>
+      <c r="G12" s="184"/>
+      <c r="H12" s="185"/>
       <c r="I12" s="115">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J12" s="182"/>
-      <c r="K12" s="183"/>
+      <c r="J12" s="186"/>
+      <c r="K12" s="187"/>
       <c r="L12" s="127"/>
       <c r="M12" s="128">
         <f>F12*I12</f>
@@ -5538,820 +5583,821 @@
       <c r="Q12" s="38"/>
       <c r="R12" s="10"/>
     </row>
-    <row r="13" spans="1:22" ht="50.1" customHeight="1" thickBot="1">
-      <c r="A13" s="197" t="s">
+    <row r="13" spans="1:22" ht="39.9" customHeight="1">
+      <c r="A13" s="181" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="182"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="183"/>
+      <c r="E13" s="182"/>
+      <c r="F13" s="126">
+        <v>0</v>
+      </c>
+      <c r="G13" s="184"/>
+      <c r="H13" s="185"/>
+      <c r="I13" s="115">
+        <v>0.02</v>
+      </c>
+      <c r="J13" s="186"/>
+      <c r="K13" s="187"/>
+      <c r="L13" s="127"/>
+      <c r="M13" s="128">
+        <f>F13*I13</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="118"/>
+      <c r="O13" s="123"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="10"/>
+    </row>
+    <row r="14" spans="1:22" ht="50.15" customHeight="1" thickBot="1">
+      <c r="A14" s="203" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="198"/>
-      <c r="C13" s="129">
+      <c r="B14" s="204"/>
+      <c r="C14" s="129">
         <f>SUM(C4:C11)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="233">
+      <c r="D14" s="239">
         <f>SUM(D4:E11)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="234"/>
-      <c r="F13" s="130">
+      <c r="E14" s="240"/>
+      <c r="F14" s="130">
         <f>SUM(F4:F12)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="252"/>
-      <c r="H13" s="253"/>
-      <c r="I13" s="131"/>
-      <c r="J13" s="237">
-        <f>SUM(J4:K12)</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="238"/>
-      <c r="L13" s="132">
-        <f>SUM(L4:L12)</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="133">
-        <f>SUM(M4:M12)</f>
-        <v>0</v>
-      </c>
-      <c r="N13" s="118"/>
-      <c r="O13" s="134"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="84"/>
-      <c r="R13" s="10"/>
-    </row>
-    <row r="14" spans="1:22" s="59" customFormat="1" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="135"/>
-      <c r="B14" s="136"/>
-      <c r="C14" s="137">
-        <v>0</v>
-      </c>
-      <c r="D14" s="138">
-        <v>0</v>
-      </c>
-      <c r="E14" s="139"/>
-      <c r="F14" s="139">
-        <v>0</v>
-      </c>
-      <c r="G14" s="140"/>
-      <c r="H14" s="141">
-        <v>0</v>
-      </c>
-      <c r="I14" s="293" t="s">
+      <c r="G14" s="258"/>
+      <c r="H14" s="259"/>
+      <c r="I14" s="131"/>
+      <c r="J14" s="243">
+        <f>SUM(J4:K13)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="244"/>
+      <c r="L14" s="132">
+        <f>SUM(L4:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="133">
+        <f>SUM(M4:M13)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="118"/>
+      <c r="O14" s="134"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="84"/>
+      <c r="R14" s="10"/>
+    </row>
+    <row r="15" spans="1:22" s="59" customFormat="1" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A15" s="135"/>
+      <c r="B15" s="136"/>
+      <c r="C15" s="137">
+        <v>0</v>
+      </c>
+      <c r="D15" s="138">
+        <v>0</v>
+      </c>
+      <c r="E15" s="139"/>
+      <c r="F15" s="139">
+        <v>0</v>
+      </c>
+      <c r="G15" s="140"/>
+      <c r="H15" s="141">
+        <v>0</v>
+      </c>
+      <c r="I15" s="295" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="294"/>
-      <c r="K14" s="295"/>
-      <c r="L14" s="142"/>
-      <c r="M14" s="143">
-        <f>L14*2%</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="144"/>
-      <c r="O14" s="144">
+      <c r="J15" s="296"/>
+      <c r="K15" s="297"/>
+      <c r="L15" s="142"/>
+      <c r="M15" s="143">
+        <f>L15*2%</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="144"/>
+      <c r="O15" s="144">
         <v>0.02</v>
       </c>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="61"/>
-    </row>
-    <row r="15" spans="1:22" ht="30" customHeight="1" thickBot="1">
-      <c r="A15" s="203" t="s">
+      <c r="P15" s="60"/>
+      <c r="Q15" s="61"/>
+    </row>
+    <row r="16" spans="1:22" ht="30" customHeight="1" thickBot="1">
+      <c r="A16" s="209" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="204"/>
-      <c r="C15" s="302" t="s">
+      <c r="B16" s="210"/>
+      <c r="C16" s="303" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="300" t="s">
+      <c r="D16" s="301" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="46"/>
-      <c r="F15" s="32" t="s">
+      <c r="E16" s="46"/>
+      <c r="F16" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G16" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H16" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="55" t="s">
+      <c r="I16" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="54"/>
-      <c r="K15" s="145"/>
-      <c r="L15" s="145"/>
-      <c r="M15" s="146"/>
-      <c r="N15" s="147">
+      <c r="J16" s="54"/>
+      <c r="K16" s="145"/>
+      <c r="L16" s="145"/>
+      <c r="M16" s="146"/>
+      <c r="N16" s="147">
         <v>1029271555.715</v>
       </c>
-      <c r="O15" s="134"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="10"/>
-      <c r="V15" s="13"/>
-    </row>
-    <row r="16" spans="1:22" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A16" s="205"/>
-      <c r="B16" s="206"/>
-      <c r="C16" s="303"/>
-      <c r="D16" s="301"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="148"/>
-      <c r="H16" s="148"/>
-      <c r="I16" s="149"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="222" t="s">
-        <v>49</v>
-      </c>
-      <c r="L16" s="223"/>
-      <c r="M16" s="150">
-        <f>M13+M14</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="151" t="s">
-        <v>45</v>
-      </c>
-      <c r="O16" s="134" t="s">
-        <v>38</v>
-      </c>
+      <c r="O16" s="134"/>
       <c r="P16" s="37"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="10"/>
-      <c r="V16" s="17"/>
-    </row>
-    <row r="17" spans="1:21" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A17" s="105" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="103" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="152"/>
-      <c r="D17" s="153">
-        <f>F4+F5-C17</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="154"/>
+      <c r="V16" s="13"/>
+    </row>
+    <row r="17" spans="1:22" ht="21.9" customHeight="1" thickBot="1">
+      <c r="A17" s="211"/>
+      <c r="B17" s="212"/>
+      <c r="C17" s="304"/>
+      <c r="D17" s="302"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G17" s="148"/>
       <c r="H17" s="148"/>
       <c r="I17" s="149"/>
       <c r="J17" s="54"/>
-      <c r="K17" s="260" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" s="261"/>
-      <c r="M17" s="155">
-        <f>(F13+L14)*1%</f>
-        <v>0</v>
-      </c>
-      <c r="N17" s="156"/>
-      <c r="O17" s="157">
-        <v>0.01</v>
+      <c r="K17" s="228" t="s">
+        <v>49</v>
+      </c>
+      <c r="L17" s="229"/>
+      <c r="M17" s="150">
+        <f>M14+M15</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="151" t="s">
+        <v>45</v>
+      </c>
+      <c r="O17" s="134" t="s">
+        <v>38</v>
       </c>
       <c r="P17" s="37"/>
       <c r="Q17" s="35"/>
       <c r="R17" s="10"/>
-    </row>
-    <row r="18" spans="1:21" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A18" s="213" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="184" t="s">
-        <v>20</v>
+      <c r="V17" s="17"/>
+    </row>
+    <row r="18" spans="1:22" ht="21.9" customHeight="1" thickBot="1">
+      <c r="A18" s="105" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="103" t="s">
+        <v>18</v>
       </c>
       <c r="C18" s="152"/>
       <c r="D18" s="153">
-        <f>F6-C18</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="158" t="s">
-        <v>56</v>
-      </c>
+        <f>F4+F5-C18</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="154"/>
       <c r="F18" s="51" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G18" s="148"/>
       <c r="H18" s="148"/>
       <c r="I18" s="149"/>
       <c r="J18" s="54"/>
-      <c r="K18" s="260" t="s">
-        <v>51</v>
-      </c>
-      <c r="L18" s="261"/>
+      <c r="K18" s="262" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" s="263"/>
       <c r="M18" s="155">
-        <f>F11</f>
-        <v>0</v>
-      </c>
-      <c r="N18" s="145"/>
-      <c r="O18" s="159"/>
+        <f>(F14+L15)*1%</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="156"/>
+      <c r="O18" s="157">
+        <v>0.01</v>
+      </c>
       <c r="P18" s="37"/>
       <c r="Q18" s="35"/>
       <c r="R18" s="10"/>
     </row>
-    <row r="19" spans="1:21" ht="21.9" customHeight="1">
-      <c r="A19" s="213"/>
-      <c r="B19" s="184"/>
+    <row r="19" spans="1:22" ht="21.9" customHeight="1" thickBot="1">
+      <c r="A19" s="219" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="190" t="s">
+        <v>20</v>
+      </c>
       <c r="C19" s="152"/>
       <c r="D19" s="153">
-        <f t="shared" ref="D19:D23" si="5">F7-C19</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="158"/>
-      <c r="F19" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" s="160">
-        <f>SUM(G16:G18)</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="160">
-        <f>SUM(H16:H18)</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="160">
-        <f>SUM(I16:I18)</f>
-        <v>0</v>
-      </c>
+        <f t="shared" ref="D19:D25" si="5">F6-C19</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="158" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="148"/>
+      <c r="H19" s="148"/>
+      <c r="I19" s="149"/>
       <c r="J19" s="54"/>
-      <c r="K19" s="111"/>
-      <c r="L19" s="111"/>
-      <c r="M19" s="111"/>
-      <c r="N19" s="159"/>
+      <c r="K19" s="262" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" s="263"/>
+      <c r="M19" s="155">
+        <f>F11</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="145"/>
       <c r="O19" s="159"/>
       <c r="P19" s="37"/>
       <c r="Q19" s="35"/>
       <c r="R19" s="10"/>
     </row>
-    <row r="20" spans="1:21" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A20" s="213"/>
-      <c r="B20" s="184"/>
+    <row r="20" spans="1:22" ht="21.9" customHeight="1">
+      <c r="A20" s="219"/>
+      <c r="B20" s="190"/>
       <c r="C20" s="152"/>
       <c r="D20" s="153">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E20" s="158"/>
-      <c r="F20" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="297">
-        <f>SUM(G19:I19)</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="298"/>
-      <c r="I20" s="299"/>
+      <c r="F20" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="160">
+        <f>SUM(G17:G19)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="160">
+        <f>SUM(H17:H19)</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="160">
+        <f>SUM(I17:I19)</f>
+        <v>0</v>
+      </c>
       <c r="J20" s="54"/>
       <c r="K20" s="111"/>
       <c r="L20" s="111"/>
       <c r="M20" s="111"/>
       <c r="N20" s="159"/>
-      <c r="O20" s="161"/>
-      <c r="P20" s="87"/>
+      <c r="O20" s="159"/>
+      <c r="P20" s="37"/>
       <c r="Q20" s="35"/>
       <c r="R20" s="10"/>
     </row>
-    <row r="21" spans="1:21" ht="29.4" customHeight="1" thickBot="1">
-      <c r="A21" s="105" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="103" t="s">
-        <v>22</v>
-      </c>
+    <row r="21" spans="1:22" ht="21.9" customHeight="1" thickBot="1">
+      <c r="A21" s="219"/>
+      <c r="B21" s="190"/>
       <c r="C21" s="152"/>
       <c r="D21" s="153">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E21" s="162" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="159"/>
-      <c r="G21" s="111"/>
-      <c r="H21" s="163"/>
-      <c r="I21" s="164">
-        <v>0</v>
-      </c>
-      <c r="J21" s="163"/>
-      <c r="K21" s="163"/>
+      <c r="E21" s="158"/>
+      <c r="F21" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="298">
+        <f>SUM(G20:I20)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="299"/>
+      <c r="I21" s="300"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="111"/>
       <c r="L21" s="111"/>
       <c r="M21" s="111"/>
-      <c r="N21" s="165"/>
-      <c r="O21" s="166"/>
-      <c r="P21" s="83"/>
+      <c r="N21" s="159"/>
+      <c r="O21" s="161"/>
+      <c r="P21" s="87"/>
       <c r="Q21" s="35"/>
       <c r="R21" s="10"/>
     </row>
-    <row r="22" spans="1:21" ht="19.5" customHeight="1" thickTop="1">
+    <row r="22" spans="1:22" ht="29.4" customHeight="1" thickBot="1">
       <c r="A22" s="105" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" s="103" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="167"/>
+        <v>22</v>
+      </c>
+      <c r="C22" s="152"/>
       <c r="D22" s="153">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E22" s="154"/>
-      <c r="F22" s="185" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="264" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" s="265"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="258" t="s">
-        <v>32</v>
-      </c>
-      <c r="L22" s="259"/>
-      <c r="M22" s="266" t="s">
-        <v>64</v>
-      </c>
+      <c r="E22" s="162" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="159"/>
+      <c r="G22" s="111"/>
+      <c r="H22" s="163"/>
+      <c r="I22" s="164">
+        <v>0</v>
+      </c>
+      <c r="J22" s="163"/>
+      <c r="K22" s="163"/>
+      <c r="L22" s="111"/>
+      <c r="M22" s="111"/>
       <c r="N22" s="165"/>
-      <c r="O22" s="263"/>
-      <c r="P22" s="262"/>
+      <c r="O22" s="166"/>
+      <c r="P22" s="83"/>
       <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-    </row>
-    <row r="23" spans="1:21" ht="38.4" customHeight="1">
+      <c r="R22" s="10"/>
+    </row>
+    <row r="23" spans="1:22" ht="19.5" customHeight="1" thickTop="1">
       <c r="A23" s="105" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="103" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="152"/>
+        <v>8</v>
+      </c>
+      <c r="C23" s="167"/>
       <c r="D23" s="153">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E23" s="154"/>
-      <c r="F23" s="186"/>
-      <c r="G23" s="100" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" s="168">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="I23" s="101"/>
-      <c r="J23" s="106"/>
-      <c r="K23" s="102" t="s">
-        <v>31</v>
-      </c>
-      <c r="L23" s="169">
-        <v>0.01</v>
-      </c>
-      <c r="M23" s="267"/>
+      <c r="F23" s="191" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="266" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="267"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="260" t="s">
+        <v>32</v>
+      </c>
+      <c r="L23" s="261"/>
+      <c r="M23" s="268" t="s">
+        <v>64</v>
+      </c>
       <c r="N23" s="165"/>
-      <c r="O23" s="263"/>
-      <c r="P23" s="262"/>
-      <c r="Q23" s="22"/>
-      <c r="S23" s="37"/>
-      <c r="U23" s="4"/>
-    </row>
-    <row r="24" spans="1:21" ht="27.6" customHeight="1" thickBot="1">
-      <c r="A24" s="197" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="198"/>
+      <c r="O23" s="265"/>
+      <c r="P23" s="264"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+    </row>
+    <row r="24" spans="1:22" ht="38.4" customHeight="1">
+      <c r="A24" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="103" t="s">
+        <v>3</v>
+      </c>
       <c r="C24" s="152"/>
       <c r="D24" s="153">
-        <f>F12-C24</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E24" s="154"/>
-      <c r="F24" s="186"/>
-      <c r="G24" s="188" t="s">
+      <c r="F24" s="192"/>
+      <c r="G24" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="168">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I24" s="101"/>
+      <c r="J24" s="106"/>
+      <c r="K24" s="102" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24" s="169">
+        <v>0.01</v>
+      </c>
+      <c r="M24" s="269"/>
+      <c r="N24" s="165"/>
+      <c r="O24" s="265"/>
+      <c r="P24" s="264"/>
+      <c r="Q24" s="22"/>
+      <c r="S24" s="37"/>
+      <c r="U24" s="4"/>
+    </row>
+    <row r="25" spans="1:22" ht="27.65" customHeight="1" thickBot="1">
+      <c r="A25" s="203" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="204"/>
+      <c r="C25" s="152"/>
+      <c r="D25" s="153">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="154"/>
+      <c r="F25" s="192"/>
+      <c r="G25" s="194" t="s">
         <v>48</v>
       </c>
-      <c r="H24" s="249" t="s">
+      <c r="H25" s="255" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="271" t="s">
+      <c r="I25" s="273" t="s">
         <v>55</v>
       </c>
-      <c r="J24" s="272"/>
-      <c r="K24" s="279" t="s">
+      <c r="J25" s="274"/>
+      <c r="K25" s="281" t="s">
         <v>52</v>
       </c>
-      <c r="L24" s="246" t="s">
+      <c r="L25" s="252" t="s">
         <v>53</v>
       </c>
-      <c r="M24" s="217">
-        <f>G28+L28+(L14*1%)</f>
-        <v>0</v>
-      </c>
-      <c r="N24" s="165"/>
-      <c r="O24" s="170"/>
-      <c r="P24" s="88"/>
-      <c r="Q24" s="4"/>
-      <c r="S24" s="35"/>
-    </row>
-    <row r="25" spans="1:21" ht="20.25" customHeight="1">
-      <c r="A25" s="287" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="288"/>
-      <c r="C25" s="268">
-        <f>SUM(C17:C24)</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="224">
-        <f>SUM(D17:D24)</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="154"/>
-      <c r="F25" s="186"/>
-      <c r="G25" s="189"/>
-      <c r="H25" s="250"/>
-      <c r="I25" s="273"/>
-      <c r="J25" s="274"/>
-      <c r="K25" s="280"/>
-      <c r="L25" s="247"/>
-      <c r="M25" s="218"/>
+      <c r="M25" s="223">
+        <f>G29+L29+(L15*1%)</f>
+        <v>0</v>
+      </c>
       <c r="N25" s="165"/>
-      <c r="O25" s="171"/>
-      <c r="P25" s="89"/>
+      <c r="O25" s="170"/>
+      <c r="P25" s="88"/>
       <c r="Q25" s="4"/>
       <c r="S25" s="35"/>
     </row>
-    <row r="26" spans="1:21" ht="20.25" customHeight="1">
-      <c r="A26" s="289"/>
+    <row r="26" spans="1:22" ht="20.25" customHeight="1">
+      <c r="A26" s="289" t="s">
+        <v>77</v>
+      </c>
       <c r="B26" s="290"/>
-      <c r="C26" s="269"/>
-      <c r="D26" s="225"/>
+      <c r="C26" s="270">
+        <f>SUM(C18:C25)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="230">
+        <f>SUM(D18:D25)</f>
+        <v>0</v>
+      </c>
       <c r="E26" s="154"/>
-      <c r="F26" s="187"/>
-      <c r="G26" s="190"/>
-      <c r="H26" s="251"/>
+      <c r="F26" s="192"/>
+      <c r="G26" s="195"/>
+      <c r="H26" s="256"/>
       <c r="I26" s="275"/>
       <c r="J26" s="276"/>
-      <c r="K26" s="281"/>
-      <c r="L26" s="248"/>
-      <c r="M26" s="218"/>
-      <c r="N26" s="159"/>
-      <c r="O26" s="172"/>
-      <c r="P26" s="90"/>
-      <c r="Q26" s="81"/>
+      <c r="K26" s="282"/>
+      <c r="L26" s="253"/>
+      <c r="M26" s="224"/>
+      <c r="N26" s="165"/>
+      <c r="O26" s="171"/>
+      <c r="P26" s="89"/>
+      <c r="Q26" s="4"/>
       <c r="S26" s="35"/>
     </row>
-    <row r="27" spans="1:21" ht="27.75" customHeight="1" thickBot="1">
+    <row r="27" spans="1:22" ht="20.25" customHeight="1">
       <c r="A27" s="291"/>
       <c r="B27" s="292"/>
-      <c r="C27" s="270"/>
-      <c r="D27" s="226"/>
+      <c r="C27" s="271"/>
+      <c r="D27" s="231"/>
       <c r="E27" s="154"/>
-      <c r="F27" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" s="173"/>
-      <c r="H27" s="174">
-        <v>0</v>
-      </c>
-      <c r="I27" s="199"/>
-      <c r="J27" s="200"/>
-      <c r="K27" s="175"/>
-      <c r="L27" s="176"/>
-      <c r="M27" s="218"/>
+      <c r="F27" s="193"/>
+      <c r="G27" s="196"/>
+      <c r="H27" s="257"/>
+      <c r="I27" s="277"/>
+      <c r="J27" s="278"/>
+      <c r="K27" s="283"/>
+      <c r="L27" s="254"/>
+      <c r="M27" s="224"/>
       <c r="N27" s="159"/>
-      <c r="O27" s="177"/>
+      <c r="O27" s="172"/>
       <c r="P27" s="90"/>
       <c r="Q27" s="81"/>
-      <c r="R27" s="35"/>
-    </row>
-    <row r="28" spans="1:21" ht="24.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A28" s="46"/>
-      <c r="B28" s="178"/>
-      <c r="C28" s="154"/>
-      <c r="D28" s="154"/>
+      <c r="S27" s="35"/>
+    </row>
+    <row r="28" spans="1:22" ht="27.75" customHeight="1" thickBot="1">
+      <c r="A28" s="293"/>
+      <c r="B28" s="294"/>
+      <c r="C28" s="272"/>
+      <c r="D28" s="232"/>
       <c r="E28" s="154"/>
-      <c r="F28" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="G28" s="277">
-        <f>(G27+H27)*H23</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="278"/>
-      <c r="I28" s="220"/>
-      <c r="J28" s="221"/>
-      <c r="K28" s="179"/>
-      <c r="L28" s="180">
-        <f>(I27+K27+L27)*L23</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="219"/>
+      <c r="F28" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="173"/>
+      <c r="H28" s="174">
+        <v>0</v>
+      </c>
+      <c r="I28" s="205"/>
+      <c r="J28" s="206"/>
+      <c r="K28" s="175"/>
+      <c r="L28" s="176"/>
+      <c r="M28" s="224"/>
       <c r="N28" s="159"/>
-      <c r="O28" s="92"/>
-      <c r="P28" s="92"/>
+      <c r="O28" s="177"/>
+      <c r="P28" s="90"/>
       <c r="Q28" s="81"/>
       <c r="R28" s="35"/>
     </row>
-    <row r="29" spans="1:21" ht="19.8" customHeight="1" thickTop="1">
+    <row r="29" spans="1:22" ht="24.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A29" s="46"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="75"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="74"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="74"/>
-      <c r="O29" s="91"/>
+      <c r="B29" s="178"/>
+      <c r="C29" s="154"/>
+      <c r="D29" s="154"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="279">
+        <f>(G28+H28)*H24</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="280"/>
+      <c r="I29" s="226"/>
+      <c r="J29" s="227"/>
+      <c r="K29" s="179"/>
+      <c r="L29" s="180">
+        <f>(I28+K28+L28)*L24</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="225"/>
+      <c r="N29" s="159"/>
+      <c r="O29" s="92"/>
       <c r="P29" s="92"/>
-      <c r="Q29" s="82"/>
+      <c r="Q29" s="81"/>
       <c r="R29" s="35"/>
     </row>
-    <row r="30" spans="1:21" ht="34.5" customHeight="1">
+    <row r="30" spans="1:22" ht="19.75" customHeight="1" thickTop="1">
       <c r="A30" s="46"/>
-      <c r="B30" s="181" t="str">
-        <f>A40&amp;M16/1000000&amp;D37&amp;B40&amp;CHAR(10)&amp;A41&amp;M24/1000000&amp;B41&amp;CHAR(10)&amp;A42&amp;"???"&amp;B42&amp;CHAR(10)&amp;A43&amp;"???"&amp;B43&amp;M24/1000000&amp;C43&amp;CHAR(10)&amp;A44</f>
-        <v>一、依放款資產評估辦法三項標準評估後，以五類資產評估 (Ａ)金額0百萬元為高。
-二、依金管會104年07月24日金管保財字第10402506096號令備抵損失提存比率為放款餘額 1.5%評估金額為 0百萬元。
-三、IFRS 9預期損失金額依據放款各相關權責單位：PD違約機率（放款審查課）、LGD違約損失率（放款管理課）、EAD曝險額（放款服務課）提供相關數據，並由放款服務課於預期損失計算系統完成核帳後，計算所得之預期損失金額為???百萬元。
-四、公司備抵損失至108 年03月實際提列???百萬元，較最高『IFRS9預期損失金額0百萬元』相比，提列金額尚足。
-五、陳核。</v>
-      </c>
-      <c r="C30" s="181"/>
-      <c r="D30" s="181"/>
-      <c r="E30" s="181"/>
-      <c r="F30" s="181"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="63"/>
-      <c r="O30" s="93"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="74"/>
+      <c r="M30" s="74"/>
+      <c r="N30" s="74"/>
+      <c r="O30" s="91"/>
       <c r="P30" s="92"/>
       <c r="Q30" s="82"/>
       <c r="R30" s="35"/>
     </row>
-    <row r="31" spans="1:21" s="40" customFormat="1" ht="160.5" customHeight="1">
-      <c r="A31" s="67" t="s">
+    <row r="31" spans="1:22" ht="34.5" customHeight="1">
+      <c r="A31" s="46"/>
+      <c r="B31" s="189" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="189"/>
+      <c r="D31" s="189"/>
+      <c r="E31" s="189"/>
+      <c r="F31" s="189"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="93"/>
+      <c r="P31" s="92"/>
+      <c r="Q31" s="82"/>
+      <c r="R31" s="35"/>
+    </row>
+    <row r="32" spans="1:22" s="40" customFormat="1" ht="160.5" customHeight="1">
+      <c r="A32" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="181"/>
-      <c r="C31" s="181"/>
-      <c r="D31" s="181"/>
-      <c r="E31" s="181"/>
-      <c r="F31" s="181"/>
-      <c r="G31" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="H31" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="I31" s="80"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="66" t="s">
+      <c r="B32" s="189"/>
+      <c r="C32" s="189"/>
+      <c r="D32" s="189"/>
+      <c r="E32" s="189"/>
+      <c r="F32" s="189"/>
+      <c r="G32" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="H32" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" s="80"/>
+      <c r="K32" s="188" t="s">
         <v>43</v>
       </c>
-      <c r="M31" s="66"/>
-      <c r="N31" s="62"/>
-      <c r="O31" s="94"/>
-      <c r="P31" s="95"/>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
-    </row>
-    <row r="32" spans="1:21" ht="31.5" hidden="1" customHeight="1">
-      <c r="A32" s="2">
+      <c r="L32" s="188"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="62"/>
+      <c r="O32" s="94"/>
+      <c r="P32" s="95"/>
+      <c r="Q32" s="45"/>
+      <c r="R32" s="45"/>
+    </row>
+    <row r="33" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+      <c r="A33" s="2">
         <v>19886411</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B33" s="2">
         <v>419490558</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C33" s="2">
         <v>4472214615</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D33" s="2">
         <v>53854214514</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2" t="e">
+      <c r="E33" s="2"/>
+      <c r="F33" s="2" t="e">
         <v>#REF!</v>
       </c>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="21"/>
-    </row>
-    <row r="33" spans="1:14" ht="31.5" hidden="1" customHeight="1">
-      <c r="A33" s="8" t="s">
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="21"/>
+    </row>
+    <row r="34" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+      <c r="A34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C34" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8" t="s">
+      <c r="E34" s="8"/>
+      <c r="F34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G33" s="39" t="s">
+      <c r="G34" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="40"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="42" t="s">
+      <c r="H34" s="40"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="L33" s="43"/>
-      <c r="M33" s="44"/>
-      <c r="N33" s="4"/>
-    </row>
-    <row r="34" spans="1:14" ht="31.5" hidden="1" customHeight="1">
-      <c r="A34" s="14" t="e">
+      <c r="L34" s="43"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+      <c r="A35" s="14" t="e">
         <v>#REF!</v>
       </c>
-      <c r="B34" s="14" t="e">
+      <c r="B35" s="14" t="e">
         <v>#REF!</v>
       </c>
-      <c r="C34" s="15" t="e">
+      <c r="C35" s="15" t="e">
         <v>#REF!</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D35" s="15">
         <v>53854214514</v>
       </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="16" t="e">
+      <c r="E35" s="15"/>
+      <c r="F35" s="16" t="e">
         <v>#REF!</v>
       </c>
-      <c r="G34" s="28" t="s">
+      <c r="G35" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="21"/>
-      <c r="I34" s="4"/>
-      <c r="K34" s="29" t="s">
+      <c r="H35" s="21"/>
+      <c r="I35" s="4"/>
+      <c r="K35" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="L34" s="1"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-    </row>
-    <row r="35" spans="1:14" ht="31.5" hidden="1" customHeight="1">
-      <c r="A35" s="5" t="e">
+      <c r="L35" s="1"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+    </row>
+    <row r="36" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+      <c r="A36" s="5" t="e">
         <v>#REF!</v>
       </c>
-      <c r="B35" s="5" t="e">
+      <c r="B36" s="5" t="e">
         <v>#REF!</v>
       </c>
-      <c r="C35" s="11" t="e">
+      <c r="C36" s="11" t="e">
         <v>#REF!</v>
       </c>
-      <c r="D35" s="11">
-        <v>0</v>
-      </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11" t="e">
+      <c r="D36" s="11">
+        <v>0</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11" t="e">
         <v>#REF!</v>
       </c>
-      <c r="G35" s="24"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="1:14" ht="31.5" hidden="1" customHeight="1">
-      <c r="C36" s="13" t="e">
+      <c r="G36" s="24"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+      <c r="C37" s="13" t="e">
         <v>#REF!</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F37" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="23"/>
-      <c r="H36" s="24"/>
-    </row>
-    <row r="37" spans="1:14" ht="31.5" customHeight="1">
-      <c r="B37" s="10" t="s">
+      <c r="G37" s="23"/>
+      <c r="H37" s="24"/>
+    </row>
+    <row r="38" spans="1:14" ht="31.5" customHeight="1">
+      <c r="B38" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="11"/>
-      <c r="H37" s="10"/>
-    </row>
-    <row r="38" spans="1:14" ht="31.5" customHeight="1">
-      <c r="C38" s="34"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A39" s="34" t="s">
-        <v>86</v>
-      </c>
+      <c r="C39" s="34"/>
     </row>
     <row r="40" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="A40" s="34"/>
+    </row>
+    <row r="41" spans="1:14" ht="31.5" customHeight="1">
+      <c r="A41"/>
+      <c r="B41" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A41" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" t="s">
-        <v>82</v>
-      </c>
-    </row>
     <row r="42" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A42" s="98" t="s">
-        <v>83</v>
-      </c>
+      <c r="A42"/>
       <c r="B42" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A43" s="98" t="s">
-        <v>84</v>
-      </c>
+      <c r="A43" s="98"/>
       <c r="B43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="31.5" customHeight="1">
+      <c r="A44" s="98"/>
+      <c r="B44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" ht="31.5" customHeight="1">
-      <c r="B49"/>
+    </row>
+    <row r="45" spans="1:14" ht="31.5" customHeight="1">
+      <c r="A45"/>
+    </row>
+    <row r="50" spans="2:2" ht="31.5" customHeight="1">
+      <c r="B50"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="I24:J26"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A25:B27"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G13:H13"/>
+  <mergeCells count="78">
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="G21:I21"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="G12:H12"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M24:M28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="M25:M29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="D26:D28"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:H3"/>
-    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="L25:L27"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="D9:E9"/>
@@ -6364,22 +6410,38 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="B30:F31"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="B6:B8"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="G25:G27"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="B31:F32"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="I25:J27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="A26:B28"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -6398,12 +6460,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="98" customWidth="1"/>
-    <col min="2" max="2" width="79.5546875" customWidth="1"/>
+    <col min="2" max="2" width="79.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="297" customHeight="1">
@@ -6420,7 +6484,7 @@
         <v>1029.31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.2" customHeight="1">
+    <row r="2" spans="1:5" ht="16.25" customHeight="1">
       <c r="A2" s="97"/>
       <c r="B2" s="97"/>
       <c r="C2" s="97"/>
@@ -6448,7 +6512,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="64.8">
+    <row r="8" spans="1:5" ht="51">
       <c r="B8" s="98" t="s">
         <v>83</v>
       </c>
@@ -6487,29 +6551,29 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.33203125" defaultRowHeight="31.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="13.36328125" defaultRowHeight="31.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="27.77734375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="27.44140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="3.44140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="20.77734375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.90625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="25.6328125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="3.08984375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="27.81640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27.453125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="27.453125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="3.453125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="20.81640625" style="4" customWidth="1"/>
     <col min="12" max="12" width="24" style="4" customWidth="1"/>
-    <col min="13" max="13" width="27.109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="6.44140625" style="10" customWidth="1"/>
-    <col min="15" max="15" width="24.21875" style="10" customWidth="1"/>
-    <col min="16" max="16" width="10.21875" style="10" customWidth="1"/>
-    <col min="17" max="17" width="20.44140625" style="37" customWidth="1"/>
-    <col min="18" max="18" width="8.77734375" style="37" customWidth="1"/>
+    <col min="13" max="13" width="27.08984375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="6.453125" style="10" customWidth="1"/>
+    <col min="15" max="15" width="24.1796875" style="10" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" style="10" customWidth="1"/>
+    <col min="17" max="17" width="20.453125" style="37" customWidth="1"/>
+    <col min="18" max="18" width="8.81640625" style="37" customWidth="1"/>
     <col min="19" max="19" width="21" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" style="10" customWidth="1"/>
-    <col min="21" max="16384" width="13.33203125" style="10"/>
+    <col min="20" max="20" width="19.36328125" style="10" customWidth="1"/>
+    <col min="21" max="16384" width="13.36328125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="39.75" customHeight="1" thickBot="1">
@@ -6536,53 +6600,53 @@
       <c r="Q1" s="36"/>
       <c r="R1" s="36"/>
     </row>
-    <row r="2" spans="1:22" s="26" customFormat="1" ht="23.1" customHeight="1" thickTop="1">
-      <c r="A2" s="203" t="s">
+    <row r="2" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1" thickTop="1">
+      <c r="A2" s="209" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="204"/>
-      <c r="C2" s="207" t="s">
+      <c r="B2" s="210"/>
+      <c r="C2" s="213" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="209" t="s">
+      <c r="D2" s="215" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="204"/>
-      <c r="F2" s="227" t="s">
+      <c r="E2" s="210"/>
+      <c r="F2" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="229" t="s">
+      <c r="G2" s="235" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="230"/>
-      <c r="I2" s="239" t="s">
+      <c r="H2" s="236"/>
+      <c r="I2" s="245" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="240"/>
-      <c r="K2" s="240"/>
-      <c r="L2" s="240"/>
-      <c r="M2" s="241"/>
+      <c r="J2" s="246"/>
+      <c r="K2" s="246"/>
+      <c r="L2" s="246"/>
+      <c r="M2" s="247"/>
       <c r="N2" s="12"/>
       <c r="O2" s="112"/>
       <c r="P2" s="36"/>
       <c r="Q2" s="38"/>
     </row>
-    <row r="3" spans="1:22" s="26" customFormat="1" ht="23.1" customHeight="1">
-      <c r="A3" s="205"/>
-      <c r="B3" s="206"/>
-      <c r="C3" s="208"/>
-      <c r="D3" s="210"/>
-      <c r="E3" s="206"/>
-      <c r="F3" s="228"/>
-      <c r="G3" s="231"/>
-      <c r="H3" s="232"/>
+    <row r="3" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1">
+      <c r="A3" s="211"/>
+      <c r="B3" s="212"/>
+      <c r="C3" s="214"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="212"/>
+      <c r="F3" s="234"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="238"/>
       <c r="I3" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="235" t="s">
+      <c r="J3" s="241" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="236"/>
+      <c r="K3" s="242"/>
       <c r="L3" s="104" t="s">
         <v>73</v>
       </c>
@@ -6595,31 +6659,31 @@
       <c r="Q3" s="58"/>
     </row>
     <row r="4" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A4" s="282" t="s">
+      <c r="A4" s="284" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="284" t="s">
+      <c r="B4" s="286" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="113"/>
-      <c r="D4" s="201"/>
-      <c r="E4" s="202"/>
+      <c r="D4" s="207"/>
+      <c r="E4" s="208"/>
       <c r="F4" s="114">
         <f>SUM(C4:E4)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="211" t="s">
+      <c r="G4" s="217" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="212"/>
+      <c r="H4" s="218"/>
       <c r="I4" s="115">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J4" s="182">
+      <c r="J4" s="186">
         <f>C4*I4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="183"/>
+      <c r="K4" s="187"/>
       <c r="L4" s="116">
         <f>D4*I4</f>
         <v>0</v>
@@ -6636,27 +6700,27 @@
       <c r="T4" s="69"/>
     </row>
     <row r="5" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A5" s="283"/>
-      <c r="B5" s="285"/>
+      <c r="A5" s="285"/>
+      <c r="B5" s="287"/>
       <c r="C5" s="113"/>
-      <c r="D5" s="215"/>
-      <c r="E5" s="216"/>
+      <c r="D5" s="221"/>
+      <c r="E5" s="222"/>
       <c r="F5" s="114">
         <f t="shared" ref="F5:F11" si="0">SUM(C5:E5)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="212" t="s">
+      <c r="G5" s="218" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="286"/>
+      <c r="H5" s="288"/>
       <c r="I5" s="115">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J5" s="182">
+      <c r="J5" s="186">
         <f t="shared" ref="J5:J9" si="1">C5*I5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="183"/>
+      <c r="K5" s="187"/>
       <c r="L5" s="116">
         <f t="shared" ref="L5:L11" si="2">D5*I5</f>
         <v>0</v>
@@ -6673,31 +6737,31 @@
       <c r="T5" s="69"/>
     </row>
     <row r="6" spans="1:22" ht="46.5" customHeight="1">
-      <c r="A6" s="213" t="s">
+      <c r="A6" s="219" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="184" t="s">
+      <c r="B6" s="190" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="113"/>
-      <c r="D6" s="201"/>
-      <c r="E6" s="202"/>
+      <c r="D6" s="207"/>
+      <c r="E6" s="208"/>
       <c r="F6" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="196" t="s">
+      <c r="G6" s="202" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="214"/>
+      <c r="H6" s="220"/>
       <c r="I6" s="115">
         <v>0.02</v>
       </c>
-      <c r="J6" s="182">
+      <c r="J6" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K6" s="183"/>
+      <c r="K6" s="187"/>
       <c r="L6" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -6714,27 +6778,27 @@
       <c r="T6" s="69"/>
     </row>
     <row r="7" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A7" s="213"/>
-      <c r="B7" s="184"/>
+      <c r="A7" s="219"/>
+      <c r="B7" s="190"/>
       <c r="C7" s="121"/>
-      <c r="D7" s="242"/>
-      <c r="E7" s="243"/>
+      <c r="D7" s="248"/>
+      <c r="E7" s="249"/>
       <c r="F7" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="195" t="s">
+      <c r="G7" s="201" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="196"/>
+      <c r="H7" s="202"/>
       <c r="I7" s="115">
         <v>0.02</v>
       </c>
-      <c r="J7" s="182">
+      <c r="J7" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7" s="183"/>
+      <c r="K7" s="187"/>
       <c r="L7" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -6751,27 +6815,27 @@
       <c r="T7" s="69"/>
     </row>
     <row r="8" spans="1:22" ht="39.75" customHeight="1">
-      <c r="A8" s="213"/>
-      <c r="B8" s="184"/>
+      <c r="A8" s="219"/>
+      <c r="B8" s="190"/>
       <c r="C8" s="113"/>
-      <c r="D8" s="201"/>
-      <c r="E8" s="202"/>
+      <c r="D8" s="207"/>
+      <c r="E8" s="208"/>
       <c r="F8" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="193" t="s">
+      <c r="G8" s="199" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="194"/>
+      <c r="H8" s="200"/>
       <c r="I8" s="115">
         <v>0.02</v>
       </c>
-      <c r="J8" s="182">
+      <c r="J8" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="183"/>
+      <c r="K8" s="187"/>
       <c r="L8" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -6795,24 +6859,24 @@
         <v>22</v>
       </c>
       <c r="C9" s="113"/>
-      <c r="D9" s="191"/>
-      <c r="E9" s="192"/>
+      <c r="D9" s="197"/>
+      <c r="E9" s="198"/>
       <c r="F9" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="193" t="s">
+      <c r="G9" s="199" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="194"/>
+      <c r="H9" s="200"/>
       <c r="I9" s="122">
         <v>0.1</v>
       </c>
-      <c r="J9" s="182">
+      <c r="J9" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K9" s="183"/>
+      <c r="K9" s="187"/>
       <c r="L9" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -6836,24 +6900,24 @@
         <v>8</v>
       </c>
       <c r="C10" s="124"/>
-      <c r="D10" s="191"/>
-      <c r="E10" s="192"/>
+      <c r="D10" s="197"/>
+      <c r="E10" s="198"/>
       <c r="F10" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="193" t="s">
+      <c r="G10" s="199" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="194"/>
+      <c r="H10" s="200"/>
       <c r="I10" s="122">
         <v>0.5</v>
       </c>
-      <c r="J10" s="182">
+      <c r="J10" s="186">
         <f>C10*I10</f>
         <v>0</v>
       </c>
-      <c r="K10" s="183"/>
+      <c r="K10" s="187"/>
       <c r="L10" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -6876,24 +6940,24 @@
         <v>3</v>
       </c>
       <c r="C11" s="113"/>
-      <c r="D11" s="244"/>
-      <c r="E11" s="245"/>
+      <c r="D11" s="250"/>
+      <c r="E11" s="251"/>
       <c r="F11" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="193" t="s">
+      <c r="G11" s="199" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="194"/>
+      <c r="H11" s="200"/>
       <c r="I11" s="125">
         <v>1</v>
       </c>
-      <c r="J11" s="182">
+      <c r="J11" s="186">
         <f t="shared" ref="J11" si="4">C11*I11</f>
         <v>0</v>
       </c>
-      <c r="K11" s="183"/>
+      <c r="K11" s="187"/>
       <c r="L11" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -6909,21 +6973,21 @@
       <c r="R11" s="11"/>
     </row>
     <row r="12" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A12" s="296" t="s">
+      <c r="A12" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="255"/>
+      <c r="B12" s="182"/>
       <c r="C12" s="113"/>
-      <c r="D12" s="254"/>
-      <c r="E12" s="255"/>
+      <c r="D12" s="183"/>
+      <c r="E12" s="182"/>
       <c r="F12" s="126"/>
-      <c r="G12" s="256"/>
-      <c r="H12" s="257"/>
+      <c r="G12" s="184"/>
+      <c r="H12" s="185"/>
       <c r="I12" s="115">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J12" s="182"/>
-      <c r="K12" s="183"/>
+      <c r="J12" s="186"/>
+      <c r="K12" s="187"/>
       <c r="L12" s="127"/>
       <c r="M12" s="128">
         <f>F12*I12</f>
@@ -6935,32 +6999,32 @@
       <c r="Q12" s="38"/>
       <c r="R12" s="10"/>
     </row>
-    <row r="13" spans="1:22" ht="50.1" customHeight="1" thickBot="1">
-      <c r="A13" s="197" t="s">
+    <row r="13" spans="1:22" ht="50.15" customHeight="1" thickBot="1">
+      <c r="A13" s="203" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="198"/>
+      <c r="B13" s="204"/>
       <c r="C13" s="129">
         <f>SUM(C4:C11)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="233">
+      <c r="D13" s="239">
         <f>SUM(D4:E11)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="234"/>
+      <c r="E13" s="240"/>
       <c r="F13" s="130">
         <f>SUM(F4:F12)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="252"/>
-      <c r="H13" s="253"/>
+      <c r="G13" s="258"/>
+      <c r="H13" s="259"/>
       <c r="I13" s="131"/>
-      <c r="J13" s="237">
+      <c r="J13" s="243">
         <f>SUM(J4:K12)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="238"/>
+      <c r="K13" s="244"/>
       <c r="L13" s="132">
         <f>SUM(L4:L12)</f>
         <v>0</v>
@@ -6992,11 +7056,11 @@
       <c r="H14" s="141">
         <v>0</v>
       </c>
-      <c r="I14" s="293" t="s">
+      <c r="I14" s="295" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="294"/>
-      <c r="K14" s="295"/>
+      <c r="J14" s="296"/>
+      <c r="K14" s="297"/>
       <c r="L14" s="142"/>
       <c r="M14" s="143">
         <f>L14*2%</f>
@@ -7010,14 +7074,14 @@
       <c r="Q14" s="61"/>
     </row>
     <row r="15" spans="1:22" ht="30" customHeight="1" thickBot="1">
-      <c r="A15" s="203" t="s">
+      <c r="A15" s="209" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="204"/>
-      <c r="C15" s="302" t="s">
+      <c r="B15" s="210"/>
+      <c r="C15" s="303" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="300" t="s">
+      <c r="D15" s="301" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="46"/>
@@ -7047,10 +7111,10 @@
       <c r="V15" s="13"/>
     </row>
     <row r="16" spans="1:22" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A16" s="205"/>
-      <c r="B16" s="206"/>
-      <c r="C16" s="303"/>
-      <c r="D16" s="301"/>
+      <c r="A16" s="211"/>
+      <c r="B16" s="212"/>
+      <c r="C16" s="304"/>
+      <c r="D16" s="302"/>
       <c r="E16" s="46"/>
       <c r="F16" s="51" t="s">
         <v>75</v>
@@ -7059,10 +7123,10 @@
       <c r="H16" s="148"/>
       <c r="I16" s="149"/>
       <c r="J16" s="54"/>
-      <c r="K16" s="222" t="s">
+      <c r="K16" s="228" t="s">
         <v>49</v>
       </c>
-      <c r="L16" s="223"/>
+      <c r="L16" s="229"/>
       <c r="M16" s="150">
         <f>M13+M14</f>
         <v>0</v>
@@ -7098,10 +7162,10 @@
       <c r="H17" s="148"/>
       <c r="I17" s="149"/>
       <c r="J17" s="54"/>
-      <c r="K17" s="260" t="s">
+      <c r="K17" s="262" t="s">
         <v>50</v>
       </c>
-      <c r="L17" s="261"/>
+      <c r="L17" s="263"/>
       <c r="M17" s="155">
         <f>(F13+L14)*1%</f>
         <v>0</v>
@@ -7115,10 +7179,10 @@
       <c r="R17" s="10"/>
     </row>
     <row r="18" spans="1:21" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A18" s="213" t="s">
+      <c r="A18" s="219" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="184" t="s">
+      <c r="B18" s="190" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="152"/>
@@ -7136,10 +7200,10 @@
       <c r="H18" s="148"/>
       <c r="I18" s="149"/>
       <c r="J18" s="54"/>
-      <c r="K18" s="260" t="s">
+      <c r="K18" s="262" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="261"/>
+      <c r="L18" s="263"/>
       <c r="M18" s="155">
         <f>F11</f>
         <v>0</v>
@@ -7151,8 +7215,8 @@
       <c r="R18" s="10"/>
     </row>
     <row r="19" spans="1:21" ht="21.9" customHeight="1">
-      <c r="A19" s="213"/>
-      <c r="B19" s="184"/>
+      <c r="A19" s="219"/>
+      <c r="B19" s="190"/>
       <c r="C19" s="152"/>
       <c r="D19" s="153">
         <f t="shared" ref="D19:D23" si="5">F7-C19</f>
@@ -7185,8 +7249,8 @@
       <c r="R19" s="10"/>
     </row>
     <row r="20" spans="1:21" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A20" s="213"/>
-      <c r="B20" s="184"/>
+      <c r="A20" s="219"/>
+      <c r="B20" s="190"/>
       <c r="C20" s="152"/>
       <c r="D20" s="153">
         <f t="shared" si="5"/>
@@ -7196,12 +7260,12 @@
       <c r="F20" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="297">
+      <c r="G20" s="298">
         <f>SUM(G19:I19)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="298"/>
-      <c r="I20" s="299"/>
+      <c r="H20" s="299"/>
+      <c r="I20" s="300"/>
       <c r="J20" s="54"/>
       <c r="K20" s="111"/>
       <c r="L20" s="111"/>
@@ -7256,25 +7320,25 @@
         <v>0</v>
       </c>
       <c r="E22" s="154"/>
-      <c r="F22" s="185" t="s">
+      <c r="F22" s="191" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="264" t="s">
+      <c r="G22" s="266" t="s">
         <v>33</v>
       </c>
-      <c r="H22" s="265"/>
+      <c r="H22" s="267"/>
       <c r="I22" s="78"/>
       <c r="J22" s="79"/>
-      <c r="K22" s="258" t="s">
+      <c r="K22" s="260" t="s">
         <v>32</v>
       </c>
-      <c r="L22" s="259"/>
-      <c r="M22" s="266" t="s">
+      <c r="L22" s="261"/>
+      <c r="M22" s="268" t="s">
         <v>64</v>
       </c>
       <c r="N22" s="165"/>
-      <c r="O22" s="263"/>
-      <c r="P22" s="262"/>
+      <c r="O22" s="265"/>
+      <c r="P22" s="264"/>
       <c r="Q22" s="35"/>
       <c r="R22" s="35"/>
     </row>
@@ -7291,7 +7355,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="154"/>
-      <c r="F23" s="186"/>
+      <c r="F23" s="192"/>
       <c r="G23" s="100" t="s">
         <v>30</v>
       </c>
@@ -7306,43 +7370,43 @@
       <c r="L23" s="169">
         <v>0.01</v>
       </c>
-      <c r="M23" s="267"/>
+      <c r="M23" s="269"/>
       <c r="N23" s="165"/>
-      <c r="O23" s="263"/>
-      <c r="P23" s="262"/>
+      <c r="O23" s="265"/>
+      <c r="P23" s="264"/>
       <c r="Q23" s="22"/>
       <c r="S23" s="37"/>
       <c r="U23" s="4"/>
     </row>
-    <row r="24" spans="1:21" ht="27.6" customHeight="1" thickBot="1">
-      <c r="A24" s="197" t="s">
+    <row r="24" spans="1:21" ht="27.65" customHeight="1" thickBot="1">
+      <c r="A24" s="203" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="198"/>
+      <c r="B24" s="204"/>
       <c r="C24" s="152"/>
       <c r="D24" s="153">
         <f>F12-C24</f>
         <v>0</v>
       </c>
       <c r="E24" s="154"/>
-      <c r="F24" s="186"/>
-      <c r="G24" s="188" t="s">
+      <c r="F24" s="192"/>
+      <c r="G24" s="194" t="s">
         <v>48</v>
       </c>
-      <c r="H24" s="249" t="s">
+      <c r="H24" s="255" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="271" t="s">
+      <c r="I24" s="273" t="s">
         <v>55</v>
       </c>
-      <c r="J24" s="272"/>
-      <c r="K24" s="279" t="s">
+      <c r="J24" s="274"/>
+      <c r="K24" s="281" t="s">
         <v>52</v>
       </c>
-      <c r="L24" s="246" t="s">
+      <c r="L24" s="252" t="s">
         <v>53</v>
       </c>
-      <c r="M24" s="217">
+      <c r="M24" s="223">
         <f>G28+L28+(L14*1%)</f>
         <v>0</v>
       </c>
@@ -7353,27 +7417,27 @@
       <c r="S24" s="35"/>
     </row>
     <row r="25" spans="1:21" ht="20.25" customHeight="1">
-      <c r="A25" s="287" t="s">
+      <c r="A25" s="289" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="288"/>
-      <c r="C25" s="268">
+      <c r="B25" s="290"/>
+      <c r="C25" s="270">
         <f>SUM(C17:C24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="224">
+      <c r="D25" s="230">
         <f>SUM(D17:D24)</f>
         <v>0</v>
       </c>
       <c r="E25" s="154"/>
-      <c r="F25" s="186"/>
-      <c r="G25" s="189"/>
-      <c r="H25" s="250"/>
-      <c r="I25" s="273"/>
-      <c r="J25" s="274"/>
-      <c r="K25" s="280"/>
-      <c r="L25" s="247"/>
-      <c r="M25" s="218"/>
+      <c r="F25" s="192"/>
+      <c r="G25" s="195"/>
+      <c r="H25" s="256"/>
+      <c r="I25" s="275"/>
+      <c r="J25" s="276"/>
+      <c r="K25" s="282"/>
+      <c r="L25" s="253"/>
+      <c r="M25" s="224"/>
       <c r="N25" s="165"/>
       <c r="O25" s="171"/>
       <c r="P25" s="89"/>
@@ -7381,19 +7445,19 @@
       <c r="S25" s="35"/>
     </row>
     <row r="26" spans="1:21" ht="20.25" customHeight="1">
-      <c r="A26" s="289"/>
-      <c r="B26" s="290"/>
-      <c r="C26" s="269"/>
-      <c r="D26" s="225"/>
+      <c r="A26" s="291"/>
+      <c r="B26" s="292"/>
+      <c r="C26" s="271"/>
+      <c r="D26" s="231"/>
       <c r="E26" s="154"/>
-      <c r="F26" s="187"/>
-      <c r="G26" s="190"/>
-      <c r="H26" s="251"/>
-      <c r="I26" s="275"/>
-      <c r="J26" s="276"/>
-      <c r="K26" s="281"/>
-      <c r="L26" s="248"/>
-      <c r="M26" s="218"/>
+      <c r="F26" s="193"/>
+      <c r="G26" s="196"/>
+      <c r="H26" s="257"/>
+      <c r="I26" s="277"/>
+      <c r="J26" s="278"/>
+      <c r="K26" s="283"/>
+      <c r="L26" s="254"/>
+      <c r="M26" s="224"/>
       <c r="N26" s="159"/>
       <c r="O26" s="172"/>
       <c r="P26" s="90"/>
@@ -7401,10 +7465,10 @@
       <c r="S26" s="35"/>
     </row>
     <row r="27" spans="1:21" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A27" s="291"/>
-      <c r="B27" s="292"/>
-      <c r="C27" s="270"/>
-      <c r="D27" s="226"/>
+      <c r="A27" s="293"/>
+      <c r="B27" s="294"/>
+      <c r="C27" s="272"/>
+      <c r="D27" s="232"/>
       <c r="E27" s="154"/>
       <c r="F27" s="56" t="s">
         <v>35</v>
@@ -7413,11 +7477,11 @@
       <c r="H27" s="174">
         <v>0</v>
       </c>
-      <c r="I27" s="199"/>
-      <c r="J27" s="200"/>
+      <c r="I27" s="205"/>
+      <c r="J27" s="206"/>
       <c r="K27" s="175"/>
       <c r="L27" s="176"/>
-      <c r="M27" s="218"/>
+      <c r="M27" s="224"/>
       <c r="N27" s="159"/>
       <c r="O27" s="177"/>
       <c r="P27" s="90"/>
@@ -7433,19 +7497,19 @@
       <c r="F28" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="277">
+      <c r="G28" s="279">
         <f>(G27+H27)*H23</f>
         <v>0</v>
       </c>
-      <c r="H28" s="278"/>
-      <c r="I28" s="220"/>
-      <c r="J28" s="221"/>
+      <c r="H28" s="280"/>
+      <c r="I28" s="226"/>
+      <c r="J28" s="227"/>
       <c r="K28" s="179"/>
       <c r="L28" s="180">
         <f>(I27+K27+L27)*L23</f>
         <v>0</v>
       </c>
-      <c r="M28" s="219"/>
+      <c r="M28" s="225"/>
       <c r="N28" s="159"/>
       <c r="O28" s="92"/>
       <c r="P28" s="92"/>
@@ -7474,13 +7538,13 @@
     </row>
     <row r="30" spans="1:21" ht="34.5" customHeight="1">
       <c r="A30" s="46"/>
-      <c r="B30" s="181" t="s">
+      <c r="B30" s="189" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="181"/>
-      <c r="D30" s="181"/>
-      <c r="E30" s="181"/>
-      <c r="F30" s="181"/>
+      <c r="C30" s="189"/>
+      <c r="D30" s="189"/>
+      <c r="E30" s="189"/>
+      <c r="F30" s="189"/>
       <c r="G30" s="48"/>
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
@@ -7498,11 +7562,11 @@
       <c r="A31" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="181"/>
-      <c r="C31" s="181"/>
-      <c r="D31" s="181"/>
-      <c r="E31" s="181"/>
-      <c r="F31" s="181"/>
+      <c r="B31" s="189"/>
+      <c r="C31" s="189"/>
+      <c r="D31" s="189"/>
+      <c r="E31" s="189"/>
+      <c r="F31" s="189"/>
       <c r="G31" s="68" t="s">
         <v>41</v>
       </c>
@@ -7747,7 +7811,6 @@
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="G20:I20"/>
-    <mergeCell ref="M22:M23"/>
     <mergeCell ref="O22:O23"/>
     <mergeCell ref="P22:P23"/>
     <mergeCell ref="A24:B24"/>
@@ -7767,6 +7830,7 @@
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="I28:J28"/>
     <mergeCell ref="B30:F31"/>
+    <mergeCell ref="M22:M23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Auto-committed on 2022/04/07 週四
</commit_message>
<xml_diff>
--- a/Program/Other/LM052_底稿_放款資產分類-會計部備呆計提.xlsx
+++ b/Program/Other/LM052_底稿_放款資產分類-會計部備呆計提.xlsx
@@ -13,16 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="備呆總表" sheetId="58" r:id="rId1"/>
-    <sheet name="工作表1" sheetId="59" r:id="rId2"/>
-    <sheet name="備呆總表 (2)" sheetId="60" r:id="rId3"/>
+    <sheet name="備呆總表(原)" sheetId="60" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Database" localSheetId="0">#REF!</definedName>
-    <definedName name="_xlnm.Database" localSheetId="2">#REF!</definedName>
+    <definedName name="_xlnm.Database" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">備呆總表!$A$1:$N$32</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'備呆總表 (2)'!$A$1:$N$31</definedName>
-    <definedName name="新" localSheetId="2">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'備呆總表(原)'!$A$1:$N$31</definedName>
+    <definedName name="新" localSheetId="1">#REF!</definedName>
     <definedName name="新">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -242,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="90">
   <si>
     <t>小計</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -935,10 +934,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">   </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>五、陳核。</t>
   </si>
   <si>
@@ -1051,13 +1046,6 @@
   <si>
     <t>百萬元，較最高『IFRS9預期損失金額』相比，提列金額尚足。</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>百萬元，較最高『IFRS9預期損失金額</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>百萬元』相比，提列金額尚足。</t>
   </si>
   <si>
     <t>催收款折溢價與費用</t>
@@ -1106,7 +1094,7 @@
     <numFmt numFmtId="182" formatCode="0_ "/>
     <numFmt numFmtId="183" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="95">
+  <fonts count="95" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -3672,7 +3660,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="305">
+  <cellXfs count="302">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3957,18 +3945,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -4212,13 +4191,43 @@
     <xf numFmtId="176" fontId="71" fillId="0" borderId="35" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="74" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="40" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="71" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="71" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="21" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4227,258 +4236,273 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="33" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="26" fillId="0" borderId="31" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="26" fillId="0" borderId="62" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="54" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="24" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="55" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="93" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="93" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="93" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="71" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="71" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="76" fillId="0" borderId="66" xfId="93" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="76" fillId="0" borderId="67" xfId="93" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="60" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="77" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="78" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="21" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="48" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="80" fillId="0" borderId="32" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="80" fillId="0" borderId="82" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="83" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="84" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="85" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="21" xfId="79" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="48" xfId="79" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="21" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="48" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="21" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="48" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="34" fillId="0" borderId="0" xfId="93" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="21" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="48" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="40" fillId="0" borderId="15" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="40" fillId="0" borderId="86" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="93" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="93" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="93" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="71" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="71" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="76" fillId="0" borderId="66" xfId="93" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="76" fillId="0" borderId="67" xfId="93" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="60" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="77" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="78" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="80" fillId="0" borderId="32" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="80" fillId="0" borderId="82" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="83" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="84" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="85" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="21" xfId="79" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="48" xfId="79" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="21" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="48" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="26" fillId="0" borderId="31" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="26" fillId="0" borderId="62" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="74" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="40" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="71" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="71" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="180" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -4521,21 +4545,6 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4552,36 +4561,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="54" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="24" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="55" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5129,11 +5108,11 @@
   </sheetPr>
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:F32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.36328125" defaultRowHeight="31.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="13.36328125" defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="12.90625" style="10" customWidth="1"/>
     <col min="2" max="2" width="19.81640625" style="10" customWidth="1"/>
@@ -5158,21 +5137,21 @@
     <col min="21" max="16384" width="13.36328125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A1" s="107" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
+    <row r="1" spans="1:22" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="104" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
       <c r="M1" s="72" t="s">
         <v>46</v>
       </c>
@@ -5182,55 +5161,55 @@
       <c r="Q1" s="36"/>
       <c r="R1" s="36"/>
     </row>
-    <row r="2" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1" thickTop="1">
-      <c r="A2" s="209" t="s">
+    <row r="2" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="195" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="196"/>
+      <c r="C2" s="249" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="251" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="213" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="215" t="s">
+      <c r="E2" s="196"/>
+      <c r="F2" s="221" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="223" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="210"/>
-      <c r="F2" s="233" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="235" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="236"/>
-      <c r="I2" s="245" t="s">
+      <c r="H2" s="224"/>
+      <c r="I2" s="235" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="246"/>
-      <c r="K2" s="246"/>
-      <c r="L2" s="246"/>
-      <c r="M2" s="247"/>
+      <c r="J2" s="236"/>
+      <c r="K2" s="236"/>
+      <c r="L2" s="236"/>
+      <c r="M2" s="237"/>
       <c r="N2" s="12"/>
-      <c r="O2" s="112"/>
+      <c r="O2" s="109"/>
       <c r="P2" s="36"/>
       <c r="Q2" s="38"/>
     </row>
-    <row r="3" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1">
-      <c r="A3" s="211"/>
-      <c r="B3" s="212"/>
-      <c r="C3" s="214"/>
-      <c r="D3" s="216"/>
-      <c r="E3" s="212"/>
-      <c r="F3" s="234"/>
-      <c r="G3" s="237"/>
-      <c r="H3" s="238"/>
+    <row r="3" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="197"/>
+      <c r="B3" s="198"/>
+      <c r="C3" s="250"/>
+      <c r="D3" s="252"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="225"/>
+      <c r="H3" s="226"/>
       <c r="I3" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="241" t="s">
+      <c r="J3" s="229" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="242"/>
-      <c r="L3" s="104" t="s">
-        <v>73</v>
+      <c r="K3" s="230"/>
+      <c r="L3" s="101" t="s">
+        <v>72</v>
       </c>
       <c r="M3" s="31" t="s">
         <v>1</v>
@@ -5240,461 +5219,461 @@
       <c r="P3" s="76"/>
       <c r="Q3" s="58"/>
     </row>
-    <row r="4" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A4" s="284" t="s">
+    <row r="4" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="261" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="286" t="s">
+      <c r="B4" s="263" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="113"/>
-      <c r="D4" s="207"/>
-      <c r="E4" s="208"/>
-      <c r="F4" s="114">
+      <c r="C4" s="110"/>
+      <c r="D4" s="240"/>
+      <c r="E4" s="241"/>
+      <c r="F4" s="111">
         <f>SUM(C4:E4)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="217" t="s">
+      <c r="G4" s="253" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="218"/>
-      <c r="I4" s="115">
+      <c r="H4" s="254"/>
+      <c r="I4" s="112">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J4" s="186">
+      <c r="J4" s="231">
         <f>C4*I4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="187"/>
-      <c r="L4" s="116">
+      <c r="K4" s="232"/>
+      <c r="L4" s="113">
         <f>D4*I4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="117">
+      <c r="M4" s="114">
         <f>SUM(J4:L4)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="118"/>
-      <c r="O4" s="119"/>
+      <c r="N4" s="115"/>
+      <c r="O4" s="116"/>
       <c r="P4" s="77"/>
       <c r="Q4" s="38"/>
       <c r="R4" s="10"/>
       <c r="T4" s="69"/>
     </row>
-    <row r="5" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A5" s="285"/>
-      <c r="B5" s="287"/>
-      <c r="C5" s="113"/>
-      <c r="D5" s="221"/>
-      <c r="E5" s="222"/>
-      <c r="F5" s="114">
+    <row r="5" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="262"/>
+      <c r="B5" s="264"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="257"/>
+      <c r="E5" s="258"/>
+      <c r="F5" s="111">
         <f t="shared" ref="F5:F11" si="0">SUM(C5:E5)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="218" t="s">
+      <c r="G5" s="254" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="288"/>
-      <c r="I5" s="115">
+      <c r="H5" s="265"/>
+      <c r="I5" s="112">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J5" s="186">
+      <c r="J5" s="231">
         <f t="shared" ref="J5:J9" si="1">C5*I5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="187"/>
-      <c r="L5" s="116">
+      <c r="K5" s="232"/>
+      <c r="L5" s="113">
         <f t="shared" ref="L5:L11" si="2">D5*I5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="117">
+      <c r="M5" s="114">
         <f t="shared" ref="M5:M11" si="3">SUM(J5:L5)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="120"/>
-      <c r="O5" s="119"/>
+      <c r="N5" s="117"/>
+      <c r="O5" s="116"/>
       <c r="P5" s="77"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="10"/>
       <c r="T5" s="69"/>
     </row>
-    <row r="6" spans="1:22" ht="46.5" customHeight="1">
-      <c r="A6" s="219" t="s">
+    <row r="6" spans="1:22" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="190" t="s">
+      <c r="B6" s="199" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="207"/>
-      <c r="E6" s="208"/>
-      <c r="F6" s="114">
+      <c r="C6" s="110"/>
+      <c r="D6" s="240"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="202" t="s">
+      <c r="G6" s="255" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="220"/>
-      <c r="I6" s="115">
+      <c r="H6" s="256"/>
+      <c r="I6" s="112">
         <v>0.02</v>
       </c>
-      <c r="J6" s="186">
+      <c r="J6" s="231">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K6" s="187"/>
-      <c r="L6" s="116">
+      <c r="K6" s="232"/>
+      <c r="L6" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M6" s="117">
+      <c r="M6" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N6" s="120"/>
-      <c r="O6" s="119"/>
+      <c r="N6" s="117"/>
+      <c r="O6" s="116"/>
       <c r="P6" s="77"/>
       <c r="Q6" s="33"/>
       <c r="R6" s="11"/>
       <c r="T6" s="69"/>
     </row>
-    <row r="7" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A7" s="219"/>
-      <c r="B7" s="190"/>
-      <c r="C7" s="121"/>
-      <c r="D7" s="248"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="114">
+    <row r="7" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="208"/>
+      <c r="B7" s="199"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="238"/>
+      <c r="E7" s="239"/>
+      <c r="F7" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="201" t="s">
+      <c r="G7" s="272" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="202"/>
-      <c r="I7" s="115">
+      <c r="H7" s="255"/>
+      <c r="I7" s="112">
         <v>0.02</v>
       </c>
-      <c r="J7" s="186">
+      <c r="J7" s="231">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7" s="187"/>
-      <c r="L7" s="116">
+      <c r="K7" s="232"/>
+      <c r="L7" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M7" s="117">
+      <c r="M7" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N7" s="118"/>
-      <c r="O7" s="119"/>
+      <c r="N7" s="115"/>
+      <c r="O7" s="116"/>
       <c r="P7" s="77"/>
       <c r="Q7" s="33"/>
       <c r="R7" s="11"/>
       <c r="T7" s="69"/>
     </row>
-    <row r="8" spans="1:22" ht="39.75" customHeight="1">
-      <c r="A8" s="219"/>
-      <c r="B8" s="190"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="207"/>
-      <c r="E8" s="208"/>
-      <c r="F8" s="114">
+    <row r="8" spans="1:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="208"/>
+      <c r="B8" s="199"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="240"/>
+      <c r="E8" s="241"/>
+      <c r="F8" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="199" t="s">
+      <c r="G8" s="259" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="200"/>
-      <c r="I8" s="115">
+      <c r="H8" s="260"/>
+      <c r="I8" s="112">
         <v>0.02</v>
       </c>
-      <c r="J8" s="186">
+      <c r="J8" s="231">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="187"/>
-      <c r="L8" s="116">
+      <c r="K8" s="232"/>
+      <c r="L8" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M8" s="117">
+      <c r="M8" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N8" s="118"/>
-      <c r="O8" s="119"/>
+      <c r="N8" s="115"/>
+      <c r="O8" s="116"/>
       <c r="P8" s="77"/>
       <c r="Q8" s="33"/>
       <c r="R8" s="11"/>
       <c r="T8" s="69"/>
     </row>
-    <row r="9" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A9" s="105" t="s">
+    <row r="9" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="103" t="s">
+      <c r="B9" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="113"/>
-      <c r="D9" s="197"/>
-      <c r="E9" s="198"/>
-      <c r="F9" s="114">
+      <c r="C9" s="110"/>
+      <c r="D9" s="247"/>
+      <c r="E9" s="248"/>
+      <c r="F9" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="199" t="s">
+      <c r="G9" s="259" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="200"/>
-      <c r="I9" s="122">
+      <c r="H9" s="260"/>
+      <c r="I9" s="119">
         <v>0.1</v>
       </c>
-      <c r="J9" s="186">
+      <c r="J9" s="231">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K9" s="187"/>
-      <c r="L9" s="116">
+      <c r="K9" s="232"/>
+      <c r="L9" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M9" s="117">
+      <c r="M9" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N9" s="118"/>
-      <c r="O9" s="123"/>
+      <c r="N9" s="115"/>
+      <c r="O9" s="120"/>
       <c r="P9" s="77"/>
       <c r="Q9" s="33"/>
       <c r="R9" s="11"/>
       <c r="T9" s="69"/>
     </row>
-    <row r="10" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A10" s="105" t="s">
+    <row r="10" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="124"/>
-      <c r="D10" s="197"/>
-      <c r="E10" s="198"/>
-      <c r="F10" s="114">
+      <c r="C10" s="121"/>
+      <c r="D10" s="247"/>
+      <c r="E10" s="248"/>
+      <c r="F10" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="199" t="s">
+      <c r="G10" s="259" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="200"/>
-      <c r="I10" s="122">
+      <c r="H10" s="260"/>
+      <c r="I10" s="119">
         <v>0.5</v>
       </c>
-      <c r="J10" s="186">
+      <c r="J10" s="231">
         <f>C10*I10</f>
         <v>0</v>
       </c>
-      <c r="K10" s="187"/>
-      <c r="L10" s="116">
+      <c r="K10" s="232"/>
+      <c r="L10" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M10" s="117">
+      <c r="M10" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N10" s="118"/>
-      <c r="O10" s="123"/>
+      <c r="N10" s="115"/>
+      <c r="O10" s="120"/>
       <c r="P10" s="77"/>
       <c r="Q10" s="33"/>
       <c r="R10" s="11"/>
     </row>
-    <row r="11" spans="1:22" ht="66.900000000000006" customHeight="1">
-      <c r="A11" s="105" t="s">
+    <row r="11" spans="1:22" ht="66.900000000000006" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="113"/>
-      <c r="D11" s="250"/>
-      <c r="E11" s="251"/>
-      <c r="F11" s="114">
+      <c r="C11" s="110"/>
+      <c r="D11" s="242"/>
+      <c r="E11" s="243"/>
+      <c r="F11" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="199" t="s">
+      <c r="G11" s="259" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="200"/>
-      <c r="I11" s="125">
+      <c r="H11" s="260"/>
+      <c r="I11" s="122">
         <v>1</v>
       </c>
-      <c r="J11" s="186">
+      <c r="J11" s="231">
         <f t="shared" ref="J11" si="4">C11*I11</f>
         <v>0</v>
       </c>
-      <c r="K11" s="187"/>
-      <c r="L11" s="116">
+      <c r="K11" s="232"/>
+      <c r="L11" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M11" s="117">
+      <c r="M11" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N11" s="118"/>
-      <c r="O11" s="123"/>
+      <c r="N11" s="115"/>
+      <c r="O11" s="120"/>
       <c r="P11" s="77"/>
       <c r="Q11" s="33"/>
       <c r="R11" s="11"/>
     </row>
-    <row r="12" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A12" s="181" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="182"/>
-      <c r="C12" s="113"/>
-      <c r="D12" s="183"/>
-      <c r="E12" s="182"/>
-      <c r="F12" s="126">
-        <v>0</v>
-      </c>
-      <c r="G12" s="184"/>
-      <c r="H12" s="185"/>
-      <c r="I12" s="115">
+    <row r="12" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="203" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="190"/>
+      <c r="C12" s="110"/>
+      <c r="D12" s="189"/>
+      <c r="E12" s="190"/>
+      <c r="F12" s="123">
+        <v>0</v>
+      </c>
+      <c r="G12" s="191"/>
+      <c r="H12" s="192"/>
+      <c r="I12" s="112">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J12" s="186"/>
-      <c r="K12" s="187"/>
-      <c r="L12" s="127"/>
-      <c r="M12" s="128">
+      <c r="J12" s="231"/>
+      <c r="K12" s="232"/>
+      <c r="L12" s="124"/>
+      <c r="M12" s="125">
         <f>F12*I12</f>
         <v>0</v>
       </c>
-      <c r="N12" s="118"/>
-      <c r="O12" s="123"/>
+      <c r="N12" s="115"/>
+      <c r="O12" s="120"/>
       <c r="P12" s="85"/>
       <c r="Q12" s="38"/>
       <c r="R12" s="10"/>
     </row>
-    <row r="13" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A13" s="181" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="182"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="183"/>
-      <c r="E13" s="182"/>
-      <c r="F13" s="126">
-        <v>0</v>
-      </c>
-      <c r="G13" s="184"/>
-      <c r="H13" s="185"/>
-      <c r="I13" s="115">
+    <row r="13" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="203" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="190"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="189"/>
+      <c r="E13" s="190"/>
+      <c r="F13" s="123">
+        <v>0</v>
+      </c>
+      <c r="G13" s="191"/>
+      <c r="H13" s="192"/>
+      <c r="I13" s="112">
         <v>0.02</v>
       </c>
-      <c r="J13" s="186"/>
-      <c r="K13" s="187"/>
-      <c r="L13" s="127"/>
-      <c r="M13" s="128">
+      <c r="J13" s="231"/>
+      <c r="K13" s="232"/>
+      <c r="L13" s="124"/>
+      <c r="M13" s="125">
         <f>F13*I13</f>
         <v>0</v>
       </c>
-      <c r="N13" s="118"/>
-      <c r="O13" s="123"/>
+      <c r="N13" s="115"/>
+      <c r="O13" s="120"/>
       <c r="P13" s="85"/>
       <c r="Q13" s="38"/>
       <c r="R13" s="10"/>
     </row>
-    <row r="14" spans="1:22" ht="50.15" customHeight="1" thickBot="1">
-      <c r="A14" s="203" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="204"/>
-      <c r="C14" s="129">
+    <row r="14" spans="1:22" ht="50.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="204" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="205"/>
+      <c r="C14" s="126">
         <f>SUM(C4:C11)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="239">
+      <c r="D14" s="227">
         <f>SUM(D4:E11)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="240"/>
-      <c r="F14" s="130">
+      <c r="E14" s="228"/>
+      <c r="F14" s="127">
         <f>SUM(F4:F12)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="258"/>
-      <c r="H14" s="259"/>
-      <c r="I14" s="131"/>
-      <c r="J14" s="243">
+      <c r="G14" s="276"/>
+      <c r="H14" s="277"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="233">
         <f>SUM(J4:K13)</f>
         <v>0</v>
       </c>
-      <c r="K14" s="244"/>
-      <c r="L14" s="132">
+      <c r="K14" s="234"/>
+      <c r="L14" s="129">
         <f>SUM(L4:L13)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="133">
+      <c r="M14" s="130">
         <f>SUM(M4:M13)</f>
         <v>0</v>
       </c>
-      <c r="N14" s="118"/>
-      <c r="O14" s="134"/>
+      <c r="N14" s="115"/>
+      <c r="O14" s="131"/>
       <c r="P14" s="86"/>
       <c r="Q14" s="84"/>
       <c r="R14" s="10"/>
     </row>
-    <row r="15" spans="1:22" s="59" customFormat="1" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A15" s="135"/>
-      <c r="B15" s="136"/>
-      <c r="C15" s="137">
-        <v>0</v>
-      </c>
-      <c r="D15" s="138">
-        <v>0</v>
-      </c>
-      <c r="E15" s="139"/>
-      <c r="F15" s="139">
-        <v>0</v>
-      </c>
-      <c r="G15" s="140"/>
-      <c r="H15" s="141">
-        <v>0</v>
-      </c>
-      <c r="I15" s="295" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="296"/>
-      <c r="K15" s="297"/>
-      <c r="L15" s="142"/>
-      <c r="M15" s="143">
+    <row r="15" spans="1:22" s="59" customFormat="1" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="132"/>
+      <c r="B15" s="133"/>
+      <c r="C15" s="134">
+        <v>0</v>
+      </c>
+      <c r="D15" s="135">
+        <v>0</v>
+      </c>
+      <c r="E15" s="136"/>
+      <c r="F15" s="136">
+        <v>0</v>
+      </c>
+      <c r="G15" s="137"/>
+      <c r="H15" s="138">
+        <v>0</v>
+      </c>
+      <c r="I15" s="200" t="s">
+        <v>79</v>
+      </c>
+      <c r="J15" s="201"/>
+      <c r="K15" s="202"/>
+      <c r="L15" s="139"/>
+      <c r="M15" s="140">
         <f>L15*2%</f>
         <v>0</v>
       </c>
-      <c r="N15" s="144"/>
-      <c r="O15" s="144">
+      <c r="N15" s="141"/>
+      <c r="O15" s="141">
         <v>0.02</v>
       </c>
       <c r="P15" s="60"/>
       <c r="Q15" s="61"/>
     </row>
-    <row r="16" spans="1:22" ht="30" customHeight="1" thickBot="1">
-      <c r="A16" s="209" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="210"/>
-      <c r="C16" s="303" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="301" t="s">
+    <row r="16" spans="1:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="195" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="196"/>
+      <c r="C16" s="209" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="206" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="46"/>
@@ -5711,43 +5690,43 @@
         <v>6</v>
       </c>
       <c r="J16" s="54"/>
-      <c r="K16" s="145"/>
-      <c r="L16" s="145"/>
-      <c r="M16" s="146"/>
-      <c r="N16" s="147">
+      <c r="K16" s="142"/>
+      <c r="L16" s="142"/>
+      <c r="M16" s="143"/>
+      <c r="N16" s="144">
         <v>1029271555.715</v>
       </c>
-      <c r="O16" s="134"/>
+      <c r="O16" s="131"/>
       <c r="P16" s="37"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="10"/>
       <c r="V16" s="13"/>
     </row>
-    <row r="17" spans="1:22" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A17" s="211"/>
-      <c r="B17" s="212"/>
-      <c r="C17" s="304"/>
-      <c r="D17" s="302"/>
+    <row r="17" spans="1:22" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="197"/>
+      <c r="B17" s="198"/>
+      <c r="C17" s="210"/>
+      <c r="D17" s="207"/>
       <c r="E17" s="46"/>
       <c r="F17" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="148"/>
-      <c r="H17" s="148"/>
-      <c r="I17" s="149"/>
+        <v>74</v>
+      </c>
+      <c r="G17" s="145"/>
+      <c r="H17" s="145"/>
+      <c r="I17" s="146"/>
       <c r="J17" s="54"/>
-      <c r="K17" s="228" t="s">
+      <c r="K17" s="216" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="229"/>
-      <c r="M17" s="150">
+      <c r="L17" s="217"/>
+      <c r="M17" s="147">
         <f>M14+M15</f>
         <v>0</v>
       </c>
-      <c r="N17" s="151" t="s">
+      <c r="N17" s="148" t="s">
         <v>45</v>
       </c>
-      <c r="O17" s="134" t="s">
+      <c r="O17" s="131" t="s">
         <v>38</v>
       </c>
       <c r="P17" s="37"/>
@@ -5755,381 +5734,381 @@
       <c r="R17" s="10"/>
       <c r="V17" s="17"/>
     </row>
-    <row r="18" spans="1:22" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A18" s="105" t="s">
+    <row r="18" spans="1:22" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="103" t="s">
+      <c r="B18" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="152"/>
-      <c r="D18" s="153">
+      <c r="C18" s="149"/>
+      <c r="D18" s="150">
         <f>F4+F5-C18</f>
         <v>0</v>
       </c>
-      <c r="E18" s="154"/>
+      <c r="E18" s="151"/>
       <c r="F18" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="148"/>
-      <c r="H18" s="148"/>
-      <c r="I18" s="149"/>
+        <v>75</v>
+      </c>
+      <c r="G18" s="145"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="146"/>
       <c r="J18" s="54"/>
-      <c r="K18" s="262" t="s">
+      <c r="K18" s="180" t="s">
         <v>50</v>
       </c>
-      <c r="L18" s="263"/>
-      <c r="M18" s="155">
+      <c r="L18" s="181"/>
+      <c r="M18" s="152">
         <f>(F14+L15)*1%</f>
         <v>0</v>
       </c>
-      <c r="N18" s="156"/>
-      <c r="O18" s="157">
+      <c r="N18" s="153"/>
+      <c r="O18" s="154">
         <v>0.01</v>
       </c>
       <c r="P18" s="37"/>
       <c r="Q18" s="35"/>
       <c r="R18" s="10"/>
     </row>
-    <row r="19" spans="1:22" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A19" s="219" t="s">
+    <row r="19" spans="1:22" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="190" t="s">
+      <c r="B19" s="199" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="152"/>
-      <c r="D19" s="153">
+      <c r="C19" s="149"/>
+      <c r="D19" s="150">
         <f t="shared" ref="D19:D25" si="5">F6-C19</f>
         <v>0</v>
       </c>
-      <c r="E19" s="158" t="s">
+      <c r="E19" s="155" t="s">
         <v>56</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" s="148"/>
-      <c r="H19" s="148"/>
-      <c r="I19" s="149"/>
+        <v>77</v>
+      </c>
+      <c r="G19" s="145"/>
+      <c r="H19" s="145"/>
+      <c r="I19" s="146"/>
       <c r="J19" s="54"/>
-      <c r="K19" s="262" t="s">
+      <c r="K19" s="180" t="s">
         <v>51</v>
       </c>
-      <c r="L19" s="263"/>
-      <c r="M19" s="155">
+      <c r="L19" s="181"/>
+      <c r="M19" s="152">
         <f>F11</f>
         <v>0</v>
       </c>
-      <c r="N19" s="145"/>
-      <c r="O19" s="159"/>
+      <c r="N19" s="142"/>
+      <c r="O19" s="156"/>
       <c r="P19" s="37"/>
       <c r="Q19" s="35"/>
       <c r="R19" s="10"/>
     </row>
-    <row r="20" spans="1:22" ht="21.9" customHeight="1">
-      <c r="A20" s="219"/>
-      <c r="B20" s="190"/>
-      <c r="C20" s="152"/>
-      <c r="D20" s="153">
+    <row r="20" spans="1:22" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="208"/>
+      <c r="B20" s="199"/>
+      <c r="C20" s="149"/>
+      <c r="D20" s="150">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E20" s="158"/>
+      <c r="E20" s="155"/>
       <c r="F20" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="160">
+      <c r="G20" s="157">
         <f>SUM(G17:G19)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="160">
+      <c r="H20" s="157">
         <f>SUM(H17:H19)</f>
         <v>0</v>
       </c>
-      <c r="I20" s="160">
+      <c r="I20" s="157">
         <f>SUM(I17:I19)</f>
         <v>0</v>
       </c>
       <c r="J20" s="54"/>
-      <c r="K20" s="111"/>
-      <c r="L20" s="111"/>
-      <c r="M20" s="111"/>
-      <c r="N20" s="159"/>
-      <c r="O20" s="159"/>
+      <c r="K20" s="108"/>
+      <c r="L20" s="108"/>
+      <c r="M20" s="108"/>
+      <c r="N20" s="156"/>
+      <c r="O20" s="156"/>
       <c r="P20" s="37"/>
       <c r="Q20" s="35"/>
       <c r="R20" s="10"/>
     </row>
-    <row r="21" spans="1:22" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A21" s="219"/>
-      <c r="B21" s="190"/>
-      <c r="C21" s="152"/>
-      <c r="D21" s="153">
+    <row r="21" spans="1:22" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="208"/>
+      <c r="B21" s="199"/>
+      <c r="C21" s="149"/>
+      <c r="D21" s="150">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E21" s="158"/>
+      <c r="E21" s="155"/>
       <c r="F21" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="298">
+      <c r="G21" s="186">
         <f>SUM(G20:I20)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="299"/>
-      <c r="I21" s="300"/>
+      <c r="H21" s="187"/>
+      <c r="I21" s="188"/>
       <c r="J21" s="54"/>
-      <c r="K21" s="111"/>
-      <c r="L21" s="111"/>
-      <c r="M21" s="111"/>
-      <c r="N21" s="159"/>
-      <c r="O21" s="161"/>
+      <c r="K21" s="108"/>
+      <c r="L21" s="108"/>
+      <c r="M21" s="108"/>
+      <c r="N21" s="156"/>
+      <c r="O21" s="158"/>
       <c r="P21" s="87"/>
       <c r="Q21" s="35"/>
       <c r="R21" s="10"/>
     </row>
-    <row r="22" spans="1:22" ht="29.4" customHeight="1" thickBot="1">
-      <c r="A22" s="105" t="s">
+    <row r="22" spans="1:22" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="152"/>
-      <c r="D22" s="153">
+      <c r="C22" s="149"/>
+      <c r="D22" s="150">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E22" s="162" t="s">
+      <c r="E22" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="159"/>
-      <c r="G22" s="111"/>
-      <c r="H22" s="163"/>
-      <c r="I22" s="164">
-        <v>0</v>
-      </c>
-      <c r="J22" s="163"/>
-      <c r="K22" s="163"/>
-      <c r="L22" s="111"/>
-      <c r="M22" s="111"/>
-      <c r="N22" s="165"/>
-      <c r="O22" s="166"/>
+      <c r="F22" s="156"/>
+      <c r="G22" s="108"/>
+      <c r="H22" s="160"/>
+      <c r="I22" s="161">
+        <v>0</v>
+      </c>
+      <c r="J22" s="160"/>
+      <c r="K22" s="160"/>
+      <c r="L22" s="108"/>
+      <c r="M22" s="108"/>
+      <c r="N22" s="162"/>
+      <c r="O22" s="163"/>
       <c r="P22" s="83"/>
       <c r="Q22" s="35"/>
       <c r="R22" s="10"/>
     </row>
-    <row r="23" spans="1:22" ht="19.5" customHeight="1" thickTop="1">
-      <c r="A23" s="105" t="s">
+    <row r="23" spans="1:22" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="103" t="s">
+      <c r="B23" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="167"/>
-      <c r="D23" s="153">
+      <c r="C23" s="164"/>
+      <c r="D23" s="150">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E23" s="154"/>
-      <c r="F23" s="191" t="s">
+      <c r="E23" s="151"/>
+      <c r="F23" s="266" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="266" t="s">
+      <c r="G23" s="182" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="267"/>
+      <c r="H23" s="183"/>
       <c r="I23" s="78"/>
       <c r="J23" s="79"/>
-      <c r="K23" s="260" t="s">
+      <c r="K23" s="193" t="s">
         <v>32</v>
       </c>
-      <c r="L23" s="261"/>
-      <c r="M23" s="268" t="s">
+      <c r="L23" s="194"/>
+      <c r="M23" s="184" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="165"/>
-      <c r="O23" s="265"/>
-      <c r="P23" s="264"/>
+      <c r="N23" s="162"/>
+      <c r="O23" s="179"/>
+      <c r="P23" s="178"/>
       <c r="Q23" s="35"/>
       <c r="R23" s="35"/>
     </row>
-    <row r="24" spans="1:22" ht="38.4" customHeight="1">
-      <c r="A24" s="105" t="s">
+    <row r="24" spans="1:22" ht="38.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="103" t="s">
+      <c r="B24" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="152"/>
-      <c r="D24" s="153">
+      <c r="C24" s="149"/>
+      <c r="D24" s="150">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E24" s="154"/>
-      <c r="F24" s="192"/>
-      <c r="G24" s="100" t="s">
+      <c r="E24" s="151"/>
+      <c r="F24" s="267"/>
+      <c r="G24" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="168">
+      <c r="H24" s="165">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I24" s="101"/>
-      <c r="J24" s="106"/>
-      <c r="K24" s="102" t="s">
+      <c r="I24" s="98"/>
+      <c r="J24" s="103"/>
+      <c r="K24" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="L24" s="169">
+      <c r="L24" s="166">
         <v>0.01</v>
       </c>
-      <c r="M24" s="269"/>
-      <c r="N24" s="165"/>
-      <c r="O24" s="265"/>
-      <c r="P24" s="264"/>
+      <c r="M24" s="185"/>
+      <c r="N24" s="162"/>
+      <c r="O24" s="179"/>
+      <c r="P24" s="178"/>
       <c r="Q24" s="22"/>
       <c r="S24" s="37"/>
       <c r="U24" s="4"/>
     </row>
-    <row r="25" spans="1:22" ht="27.65" customHeight="1" thickBot="1">
-      <c r="A25" s="203" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="204"/>
-      <c r="C25" s="152"/>
-      <c r="D25" s="153">
+    <row r="25" spans="1:22" ht="27.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="204" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="205"/>
+      <c r="C25" s="149"/>
+      <c r="D25" s="150">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E25" s="154"/>
-      <c r="F25" s="192"/>
-      <c r="G25" s="194" t="s">
+      <c r="E25" s="151"/>
+      <c r="F25" s="267"/>
+      <c r="G25" s="269" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="255" t="s">
+      <c r="H25" s="273" t="s">
         <v>54</v>
       </c>
-      <c r="I25" s="273" t="s">
+      <c r="I25" s="285" t="s">
         <v>55</v>
       </c>
-      <c r="J25" s="274"/>
-      <c r="K25" s="281" t="s">
+      <c r="J25" s="286"/>
+      <c r="K25" s="293" t="s">
         <v>52</v>
       </c>
-      <c r="L25" s="252" t="s">
+      <c r="L25" s="244" t="s">
         <v>53</v>
       </c>
-      <c r="M25" s="223">
+      <c r="M25" s="211">
         <f>G29+L29+(L15*1%)</f>
         <v>0</v>
       </c>
-      <c r="N25" s="165"/>
-      <c r="O25" s="170"/>
+      <c r="N25" s="162"/>
+      <c r="O25" s="167"/>
       <c r="P25" s="88"/>
       <c r="Q25" s="4"/>
       <c r="S25" s="35"/>
     </row>
-    <row r="26" spans="1:22" ht="20.25" customHeight="1">
-      <c r="A26" s="289" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="290"/>
-      <c r="C26" s="270">
+    <row r="26" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="296" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="297"/>
+      <c r="C26" s="282">
         <f>SUM(C18:C25)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="230">
+      <c r="D26" s="218">
         <f>SUM(D18:D25)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="154"/>
-      <c r="F26" s="192"/>
-      <c r="G26" s="195"/>
-      <c r="H26" s="256"/>
-      <c r="I26" s="275"/>
-      <c r="J26" s="276"/>
-      <c r="K26" s="282"/>
-      <c r="L26" s="253"/>
-      <c r="M26" s="224"/>
-      <c r="N26" s="165"/>
-      <c r="O26" s="171"/>
+      <c r="E26" s="151"/>
+      <c r="F26" s="267"/>
+      <c r="G26" s="270"/>
+      <c r="H26" s="274"/>
+      <c r="I26" s="287"/>
+      <c r="J26" s="288"/>
+      <c r="K26" s="294"/>
+      <c r="L26" s="245"/>
+      <c r="M26" s="212"/>
+      <c r="N26" s="162"/>
+      <c r="O26" s="168"/>
       <c r="P26" s="89"/>
       <c r="Q26" s="4"/>
       <c r="S26" s="35"/>
     </row>
-    <row r="27" spans="1:22" ht="20.25" customHeight="1">
-      <c r="A27" s="291"/>
-      <c r="B27" s="292"/>
-      <c r="C27" s="271"/>
-      <c r="D27" s="231"/>
-      <c r="E27" s="154"/>
-      <c r="F27" s="193"/>
-      <c r="G27" s="196"/>
-      <c r="H27" s="257"/>
-      <c r="I27" s="277"/>
-      <c r="J27" s="278"/>
-      <c r="K27" s="283"/>
-      <c r="L27" s="254"/>
-      <c r="M27" s="224"/>
-      <c r="N27" s="159"/>
-      <c r="O27" s="172"/>
+    <row r="27" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="298"/>
+      <c r="B27" s="299"/>
+      <c r="C27" s="283"/>
+      <c r="D27" s="219"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="268"/>
+      <c r="G27" s="271"/>
+      <c r="H27" s="275"/>
+      <c r="I27" s="289"/>
+      <c r="J27" s="290"/>
+      <c r="K27" s="295"/>
+      <c r="L27" s="246"/>
+      <c r="M27" s="212"/>
+      <c r="N27" s="156"/>
+      <c r="O27" s="169"/>
       <c r="P27" s="90"/>
       <c r="Q27" s="81"/>
       <c r="S27" s="35"/>
     </row>
-    <row r="28" spans="1:22" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A28" s="293"/>
-      <c r="B28" s="294"/>
-      <c r="C28" s="272"/>
-      <c r="D28" s="232"/>
-      <c r="E28" s="154"/>
+    <row r="28" spans="1:22" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="300"/>
+      <c r="B28" s="301"/>
+      <c r="C28" s="284"/>
+      <c r="D28" s="220"/>
+      <c r="E28" s="151"/>
       <c r="F28" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="173"/>
-      <c r="H28" s="174">
-        <v>0</v>
-      </c>
-      <c r="I28" s="205"/>
-      <c r="J28" s="206"/>
-      <c r="K28" s="175"/>
-      <c r="L28" s="176"/>
-      <c r="M28" s="224"/>
-      <c r="N28" s="159"/>
-      <c r="O28" s="177"/>
+      <c r="G28" s="170"/>
+      <c r="H28" s="171">
+        <v>0</v>
+      </c>
+      <c r="I28" s="280"/>
+      <c r="J28" s="281"/>
+      <c r="K28" s="172"/>
+      <c r="L28" s="173"/>
+      <c r="M28" s="212"/>
+      <c r="N28" s="156"/>
+      <c r="O28" s="174"/>
       <c r="P28" s="90"/>
       <c r="Q28" s="81"/>
       <c r="R28" s="35"/>
     </row>
-    <row r="29" spans="1:22" ht="24.75" customHeight="1" thickTop="1" thickBot="1">
+    <row r="29" spans="1:22" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="46"/>
-      <c r="B29" s="178"/>
-      <c r="C29" s="154"/>
-      <c r="D29" s="154"/>
-      <c r="E29" s="154"/>
+      <c r="B29" s="175"/>
+      <c r="C29" s="151"/>
+      <c r="D29" s="151"/>
+      <c r="E29" s="151"/>
       <c r="F29" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="279">
+      <c r="G29" s="291">
         <f>(G28+H28)*H24</f>
         <v>0</v>
       </c>
-      <c r="H29" s="280"/>
-      <c r="I29" s="226"/>
-      <c r="J29" s="227"/>
-      <c r="K29" s="179"/>
-      <c r="L29" s="180">
+      <c r="H29" s="292"/>
+      <c r="I29" s="214"/>
+      <c r="J29" s="215"/>
+      <c r="K29" s="176"/>
+      <c r="L29" s="177">
         <f>(I28+K28+L28)*L24</f>
         <v>0</v>
       </c>
-      <c r="M29" s="225"/>
-      <c r="N29" s="159"/>
+      <c r="M29" s="213"/>
+      <c r="N29" s="156"/>
       <c r="O29" s="92"/>
       <c r="P29" s="92"/>
       <c r="Q29" s="81"/>
       <c r="R29" s="35"/>
     </row>
-    <row r="30" spans="1:22" ht="19.75" customHeight="1" thickTop="1">
+    <row r="30" spans="1:22" ht="19.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A30" s="46"/>
       <c r="B30" s="47"/>
       <c r="C30" s="25"/>
@@ -6149,15 +6128,15 @@
       <c r="Q30" s="82"/>
       <c r="R30" s="35"/>
     </row>
-    <row r="31" spans="1:22" ht="34.5" customHeight="1">
+    <row r="31" spans="1:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="46"/>
-      <c r="B31" s="189" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="189"/>
-      <c r="D31" s="189"/>
-      <c r="E31" s="189"/>
-      <c r="F31" s="189"/>
+      <c r="B31" s="279" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="279"/>
+      <c r="D31" s="279"/>
+      <c r="E31" s="279"/>
+      <c r="F31" s="279"/>
       <c r="G31" s="48"/>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
@@ -6171,26 +6150,26 @@
       <c r="Q31" s="82"/>
       <c r="R31" s="35"/>
     </row>
-    <row r="32" spans="1:22" s="40" customFormat="1" ht="160.5" customHeight="1">
+    <row r="32" spans="1:22" s="40" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="189"/>
-      <c r="C32" s="189"/>
-      <c r="D32" s="189"/>
-      <c r="E32" s="189"/>
-      <c r="F32" s="189"/>
+      <c r="B32" s="279"/>
+      <c r="C32" s="279"/>
+      <c r="D32" s="279"/>
+      <c r="E32" s="279"/>
+      <c r="F32" s="279"/>
       <c r="G32" s="68" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H32" s="65" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I32" s="80"/>
-      <c r="K32" s="188" t="s">
+      <c r="K32" s="278" t="s">
         <v>43</v>
       </c>
-      <c r="L32" s="188"/>
+      <c r="L32" s="278"/>
       <c r="M32" s="66"/>
       <c r="N32" s="62"/>
       <c r="O32" s="94"/>
@@ -6198,7 +6177,7 @@
       <c r="Q32" s="45"/>
       <c r="R32" s="45"/>
     </row>
-    <row r="33" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+    <row r="33" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>19886411</v>
       </c>
@@ -6224,7 +6203,7 @@
       <c r="M33" s="3"/>
       <c r="N33" s="21"/>
     </row>
-    <row r="34" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+    <row r="34" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="8" t="s">
         <v>14</v>
       </c>
@@ -6254,7 +6233,7 @@
       <c r="M34" s="44"/>
       <c r="N34" s="4"/>
     </row>
-    <row r="35" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+    <row r="35" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="14" t="e">
         <v>#REF!</v>
       </c>
@@ -6283,7 +6262,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
     </row>
-    <row r="36" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+    <row r="36" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="5" t="e">
         <v>#REF!</v>
       </c>
@@ -6306,7 +6285,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+    <row r="37" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C37" s="13" t="e">
         <v>#REF!</v>
       </c>
@@ -6316,72 +6295,84 @@
       <c r="G37" s="23"/>
       <c r="H37" s="24"/>
     </row>
-    <row r="38" spans="1:14" ht="31.5" customHeight="1">
+    <row r="38" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B38" s="10" t="s">
         <v>39</v>
       </c>
       <c r="G38" s="11"/>
       <c r="H38" s="10"/>
     </row>
-    <row r="39" spans="1:14" ht="31.5" customHeight="1">
+    <row r="39" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C39" s="34"/>
     </row>
-    <row r="40" spans="1:14" ht="31.5" customHeight="1">
+    <row r="40" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="34"/>
     </row>
-    <row r="41" spans="1:14" ht="31.5" customHeight="1">
+    <row r="41" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41"/>
-      <c r="B41" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="31.5" customHeight="1">
+      <c r="B41"/>
+    </row>
+    <row r="42" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42"/>
-      <c r="B42" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A43" s="98"/>
-      <c r="B43" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A44" s="98"/>
-      <c r="B44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="34" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="31.5" customHeight="1">
+      <c r="B42"/>
+    </row>
+    <row r="43" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="96"/>
+      <c r="B43"/>
+    </row>
+    <row r="44" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="96"/>
+      <c r="B44"/>
+      <c r="C44" s="34"/>
+    </row>
+    <row r="45" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45"/>
     </row>
-    <row r="50" spans="2:2" ht="31.5" customHeight="1">
+    <row r="50" spans="2:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B50"/>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="P23:P24"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="B31:F32"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="I25:J27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="A26:B28"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="M25:M29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="K17:L17"/>
@@ -6398,50 +6389,28 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="L25:L27"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:E3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="H25:H27"/>
-    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="J13:K13"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="B31:F32"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="I25:J27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="K25:K27"/>
-    <mergeCell ref="A26:B28"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="G21:I21"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -6457,89 +6426,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
-  <cols>
-    <col min="1" max="1" width="98" customWidth="1"/>
-    <col min="2" max="2" width="79.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="297" customHeight="1">
-      <c r="A1" s="96" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="97" t="str">
-        <f>B4&amp;E1&amp;C4</f>
-        <v>一、依放款資產評估辦法三項標準評估後，以五類資產評估 (Ａ)金額1029.31百萬元為高。</v>
-      </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="99">
-        <v>1029.31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.25" customHeight="1">
-      <c r="A2" s="97"/>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="51">
-      <c r="B8" s="98" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="98" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor indexed="13"/>
@@ -6547,11 +6433,11 @@
   </sheetPr>
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.36328125" defaultRowHeight="31.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="13.36328125" defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="12.90625" style="10" customWidth="1"/>
     <col min="2" max="2" width="19.81640625" style="10" customWidth="1"/>
@@ -6576,21 +6462,21 @@
     <col min="21" max="16384" width="13.36328125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A1" s="107" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
+    <row r="1" spans="1:22" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="104" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
       <c r="M1" s="72" t="s">
         <v>46</v>
       </c>
@@ -6600,55 +6486,55 @@
       <c r="Q1" s="36"/>
       <c r="R1" s="36"/>
     </row>
-    <row r="2" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1" thickTop="1">
-      <c r="A2" s="209" t="s">
+    <row r="2" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="195" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="196"/>
+      <c r="C2" s="249" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="251" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="213" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="215" t="s">
+      <c r="E2" s="196"/>
+      <c r="F2" s="221" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="223" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="210"/>
-      <c r="F2" s="233" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="235" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="236"/>
-      <c r="I2" s="245" t="s">
+      <c r="H2" s="224"/>
+      <c r="I2" s="235" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="246"/>
-      <c r="K2" s="246"/>
-      <c r="L2" s="246"/>
-      <c r="M2" s="247"/>
+      <c r="J2" s="236"/>
+      <c r="K2" s="236"/>
+      <c r="L2" s="236"/>
+      <c r="M2" s="237"/>
       <c r="N2" s="12"/>
-      <c r="O2" s="112"/>
+      <c r="O2" s="109"/>
       <c r="P2" s="36"/>
       <c r="Q2" s="38"/>
     </row>
-    <row r="3" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1">
-      <c r="A3" s="211"/>
-      <c r="B3" s="212"/>
-      <c r="C3" s="214"/>
-      <c r="D3" s="216"/>
-      <c r="E3" s="212"/>
-      <c r="F3" s="234"/>
-      <c r="G3" s="237"/>
-      <c r="H3" s="238"/>
+    <row r="3" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="197"/>
+      <c r="B3" s="198"/>
+      <c r="C3" s="250"/>
+      <c r="D3" s="252"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="225"/>
+      <c r="H3" s="226"/>
       <c r="I3" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="241" t="s">
+      <c r="J3" s="229" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="242"/>
-      <c r="L3" s="104" t="s">
-        <v>73</v>
+      <c r="K3" s="230"/>
+      <c r="L3" s="101" t="s">
+        <v>72</v>
       </c>
       <c r="M3" s="31" t="s">
         <v>1</v>
@@ -6658,430 +6544,430 @@
       <c r="P3" s="76"/>
       <c r="Q3" s="58"/>
     </row>
-    <row r="4" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A4" s="284" t="s">
+    <row r="4" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="261" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="286" t="s">
+      <c r="B4" s="263" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="113"/>
-      <c r="D4" s="207"/>
-      <c r="E4" s="208"/>
-      <c r="F4" s="114">
+      <c r="C4" s="110"/>
+      <c r="D4" s="240"/>
+      <c r="E4" s="241"/>
+      <c r="F4" s="111">
         <f>SUM(C4:E4)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="217" t="s">
+      <c r="G4" s="253" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="218"/>
-      <c r="I4" s="115">
+      <c r="H4" s="254"/>
+      <c r="I4" s="112">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J4" s="186">
+      <c r="J4" s="231">
         <f>C4*I4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="187"/>
-      <c r="L4" s="116">
+      <c r="K4" s="232"/>
+      <c r="L4" s="113">
         <f>D4*I4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="117">
+      <c r="M4" s="114">
         <f>SUM(J4:L4)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="118"/>
-      <c r="O4" s="119"/>
+      <c r="N4" s="115"/>
+      <c r="O4" s="116"/>
       <c r="P4" s="77"/>
       <c r="Q4" s="38"/>
       <c r="R4" s="10"/>
       <c r="T4" s="69"/>
     </row>
-    <row r="5" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A5" s="285"/>
-      <c r="B5" s="287"/>
-      <c r="C5" s="113"/>
-      <c r="D5" s="221"/>
-      <c r="E5" s="222"/>
-      <c r="F5" s="114">
+    <row r="5" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="262"/>
+      <c r="B5" s="264"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="257"/>
+      <c r="E5" s="258"/>
+      <c r="F5" s="111">
         <f t="shared" ref="F5:F11" si="0">SUM(C5:E5)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="218" t="s">
+      <c r="G5" s="254" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="288"/>
-      <c r="I5" s="115">
+      <c r="H5" s="265"/>
+      <c r="I5" s="112">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J5" s="186">
+      <c r="J5" s="231">
         <f t="shared" ref="J5:J9" si="1">C5*I5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="187"/>
-      <c r="L5" s="116">
+      <c r="K5" s="232"/>
+      <c r="L5" s="113">
         <f t="shared" ref="L5:L11" si="2">D5*I5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="117">
+      <c r="M5" s="114">
         <f t="shared" ref="M5:M11" si="3">SUM(J5:L5)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="120"/>
-      <c r="O5" s="119"/>
+      <c r="N5" s="117"/>
+      <c r="O5" s="116"/>
       <c r="P5" s="77"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="10"/>
       <c r="T5" s="69"/>
     </row>
-    <row r="6" spans="1:22" ht="46.5" customHeight="1">
-      <c r="A6" s="219" t="s">
+    <row r="6" spans="1:22" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="190" t="s">
+      <c r="B6" s="199" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="207"/>
-      <c r="E6" s="208"/>
-      <c r="F6" s="114">
+      <c r="C6" s="110"/>
+      <c r="D6" s="240"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="202" t="s">
+      <c r="G6" s="255" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="220"/>
-      <c r="I6" s="115">
+      <c r="H6" s="256"/>
+      <c r="I6" s="112">
         <v>0.02</v>
       </c>
-      <c r="J6" s="186">
+      <c r="J6" s="231">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K6" s="187"/>
-      <c r="L6" s="116">
+      <c r="K6" s="232"/>
+      <c r="L6" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M6" s="117">
+      <c r="M6" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N6" s="120"/>
-      <c r="O6" s="119"/>
+      <c r="N6" s="117"/>
+      <c r="O6" s="116"/>
       <c r="P6" s="77"/>
       <c r="Q6" s="33"/>
       <c r="R6" s="11"/>
       <c r="T6" s="69"/>
     </row>
-    <row r="7" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A7" s="219"/>
-      <c r="B7" s="190"/>
-      <c r="C7" s="121"/>
-      <c r="D7" s="248"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="114">
+    <row r="7" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="208"/>
+      <c r="B7" s="199"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="238"/>
+      <c r="E7" s="239"/>
+      <c r="F7" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="201" t="s">
+      <c r="G7" s="272" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="202"/>
-      <c r="I7" s="115">
+      <c r="H7" s="255"/>
+      <c r="I7" s="112">
         <v>0.02</v>
       </c>
-      <c r="J7" s="186">
+      <c r="J7" s="231">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7" s="187"/>
-      <c r="L7" s="116">
+      <c r="K7" s="232"/>
+      <c r="L7" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M7" s="117">
+      <c r="M7" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N7" s="118"/>
-      <c r="O7" s="119"/>
+      <c r="N7" s="115"/>
+      <c r="O7" s="116"/>
       <c r="P7" s="77"/>
       <c r="Q7" s="33"/>
       <c r="R7" s="11"/>
       <c r="T7" s="69"/>
     </row>
-    <row r="8" spans="1:22" ht="39.75" customHeight="1">
-      <c r="A8" s="219"/>
-      <c r="B8" s="190"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="207"/>
-      <c r="E8" s="208"/>
-      <c r="F8" s="114">
+    <row r="8" spans="1:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="208"/>
+      <c r="B8" s="199"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="240"/>
+      <c r="E8" s="241"/>
+      <c r="F8" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="199" t="s">
+      <c r="G8" s="259" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="200"/>
-      <c r="I8" s="115">
+      <c r="H8" s="260"/>
+      <c r="I8" s="112">
         <v>0.02</v>
       </c>
-      <c r="J8" s="186">
+      <c r="J8" s="231">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="187"/>
-      <c r="L8" s="116">
+      <c r="K8" s="232"/>
+      <c r="L8" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M8" s="117">
+      <c r="M8" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N8" s="118"/>
-      <c r="O8" s="119"/>
+      <c r="N8" s="115"/>
+      <c r="O8" s="116"/>
       <c r="P8" s="77"/>
       <c r="Q8" s="33"/>
       <c r="R8" s="11"/>
       <c r="T8" s="69"/>
     </row>
-    <row r="9" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A9" s="105" t="s">
+    <row r="9" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="103" t="s">
+      <c r="B9" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="113"/>
-      <c r="D9" s="197"/>
-      <c r="E9" s="198"/>
-      <c r="F9" s="114">
+      <c r="C9" s="110"/>
+      <c r="D9" s="247"/>
+      <c r="E9" s="248"/>
+      <c r="F9" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="199" t="s">
+      <c r="G9" s="259" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="200"/>
-      <c r="I9" s="122">
+      <c r="H9" s="260"/>
+      <c r="I9" s="119">
         <v>0.1</v>
       </c>
-      <c r="J9" s="186">
+      <c r="J9" s="231">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K9" s="187"/>
-      <c r="L9" s="116">
+      <c r="K9" s="232"/>
+      <c r="L9" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M9" s="117">
+      <c r="M9" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N9" s="118"/>
-      <c r="O9" s="123"/>
+      <c r="N9" s="115"/>
+      <c r="O9" s="120"/>
       <c r="P9" s="77"/>
       <c r="Q9" s="33"/>
       <c r="R9" s="11"/>
       <c r="T9" s="69"/>
     </row>
-    <row r="10" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A10" s="105" t="s">
+    <row r="10" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="124"/>
-      <c r="D10" s="197"/>
-      <c r="E10" s="198"/>
-      <c r="F10" s="114">
+      <c r="C10" s="121"/>
+      <c r="D10" s="247"/>
+      <c r="E10" s="248"/>
+      <c r="F10" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="199" t="s">
+      <c r="G10" s="259" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="200"/>
-      <c r="I10" s="122">
+      <c r="H10" s="260"/>
+      <c r="I10" s="119">
         <v>0.5</v>
       </c>
-      <c r="J10" s="186">
+      <c r="J10" s="231">
         <f>C10*I10</f>
         <v>0</v>
       </c>
-      <c r="K10" s="187"/>
-      <c r="L10" s="116">
+      <c r="K10" s="232"/>
+      <c r="L10" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M10" s="117">
+      <c r="M10" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N10" s="118"/>
-      <c r="O10" s="123"/>
+      <c r="N10" s="115"/>
+      <c r="O10" s="120"/>
       <c r="P10" s="77"/>
       <c r="Q10" s="33"/>
       <c r="R10" s="11"/>
     </row>
-    <row r="11" spans="1:22" ht="66.900000000000006" customHeight="1">
-      <c r="A11" s="105" t="s">
+    <row r="11" spans="1:22" ht="66.900000000000006" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="113"/>
-      <c r="D11" s="250"/>
-      <c r="E11" s="251"/>
-      <c r="F11" s="114">
+      <c r="C11" s="110"/>
+      <c r="D11" s="242"/>
+      <c r="E11" s="243"/>
+      <c r="F11" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="199" t="s">
+      <c r="G11" s="259" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="200"/>
-      <c r="I11" s="125">
+      <c r="H11" s="260"/>
+      <c r="I11" s="122">
         <v>1</v>
       </c>
-      <c r="J11" s="186">
+      <c r="J11" s="231">
         <f t="shared" ref="J11" si="4">C11*I11</f>
         <v>0</v>
       </c>
-      <c r="K11" s="187"/>
-      <c r="L11" s="116">
+      <c r="K11" s="232"/>
+      <c r="L11" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M11" s="117">
+      <c r="M11" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N11" s="118"/>
-      <c r="O11" s="123"/>
+      <c r="N11" s="115"/>
+      <c r="O11" s="120"/>
       <c r="P11" s="77"/>
       <c r="Q11" s="33"/>
       <c r="R11" s="11"/>
     </row>
-    <row r="12" spans="1:22" ht="39.9" customHeight="1">
-      <c r="A12" s="181" t="s">
+    <row r="12" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="203" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="182"/>
-      <c r="C12" s="113"/>
-      <c r="D12" s="183"/>
-      <c r="E12" s="182"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="185"/>
-      <c r="I12" s="115">
+      <c r="B12" s="190"/>
+      <c r="C12" s="110"/>
+      <c r="D12" s="189"/>
+      <c r="E12" s="190"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="191"/>
+      <c r="H12" s="192"/>
+      <c r="I12" s="112">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J12" s="186"/>
-      <c r="K12" s="187"/>
-      <c r="L12" s="127"/>
-      <c r="M12" s="128">
+      <c r="J12" s="231"/>
+      <c r="K12" s="232"/>
+      <c r="L12" s="124"/>
+      <c r="M12" s="125">
         <f>F12*I12</f>
         <v>0</v>
       </c>
-      <c r="N12" s="118"/>
-      <c r="O12" s="123"/>
+      <c r="N12" s="115"/>
+      <c r="O12" s="120"/>
       <c r="P12" s="85"/>
       <c r="Q12" s="38"/>
       <c r="R12" s="10"/>
     </row>
-    <row r="13" spans="1:22" ht="50.15" customHeight="1" thickBot="1">
-      <c r="A13" s="203" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="204"/>
-      <c r="C13" s="129">
+    <row r="13" spans="1:22" ht="50.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="204" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="205"/>
+      <c r="C13" s="126">
         <f>SUM(C4:C11)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="239">
+      <c r="D13" s="227">
         <f>SUM(D4:E11)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="240"/>
-      <c r="F13" s="130">
+      <c r="E13" s="228"/>
+      <c r="F13" s="127">
         <f>SUM(F4:F12)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="258"/>
-      <c r="H13" s="259"/>
-      <c r="I13" s="131"/>
-      <c r="J13" s="243">
+      <c r="G13" s="276"/>
+      <c r="H13" s="277"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="233">
         <f>SUM(J4:K12)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="244"/>
-      <c r="L13" s="132">
+      <c r="K13" s="234"/>
+      <c r="L13" s="129">
         <f>SUM(L4:L12)</f>
         <v>0</v>
       </c>
-      <c r="M13" s="133">
+      <c r="M13" s="130">
         <f>SUM(M4:M12)</f>
         <v>0</v>
       </c>
-      <c r="N13" s="118"/>
-      <c r="O13" s="134"/>
+      <c r="N13" s="115"/>
+      <c r="O13" s="131"/>
       <c r="P13" s="86"/>
       <c r="Q13" s="84"/>
       <c r="R13" s="10"/>
     </row>
-    <row r="14" spans="1:22" s="59" customFormat="1" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="135"/>
-      <c r="B14" s="136"/>
-      <c r="C14" s="137">
-        <v>0</v>
-      </c>
-      <c r="D14" s="138">
-        <v>0</v>
-      </c>
-      <c r="E14" s="139"/>
-      <c r="F14" s="139">
-        <v>0</v>
-      </c>
-      <c r="G14" s="140"/>
-      <c r="H14" s="141">
-        <v>0</v>
-      </c>
-      <c r="I14" s="295" t="s">
-        <v>80</v>
-      </c>
-      <c r="J14" s="296"/>
-      <c r="K14" s="297"/>
-      <c r="L14" s="142"/>
-      <c r="M14" s="143">
+    <row r="14" spans="1:22" s="59" customFormat="1" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="132"/>
+      <c r="B14" s="133"/>
+      <c r="C14" s="134">
+        <v>0</v>
+      </c>
+      <c r="D14" s="135">
+        <v>0</v>
+      </c>
+      <c r="E14" s="136"/>
+      <c r="F14" s="136">
+        <v>0</v>
+      </c>
+      <c r="G14" s="137"/>
+      <c r="H14" s="138">
+        <v>0</v>
+      </c>
+      <c r="I14" s="200" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="201"/>
+      <c r="K14" s="202"/>
+      <c r="L14" s="139"/>
+      <c r="M14" s="140">
         <f>L14*2%</f>
         <v>0</v>
       </c>
-      <c r="N14" s="144"/>
-      <c r="O14" s="144">
+      <c r="N14" s="141"/>
+      <c r="O14" s="141">
         <v>0.02</v>
       </c>
       <c r="P14" s="60"/>
       <c r="Q14" s="61"/>
     </row>
-    <row r="15" spans="1:22" ht="30" customHeight="1" thickBot="1">
-      <c r="A15" s="209" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="210"/>
-      <c r="C15" s="303" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="301" t="s">
+    <row r="15" spans="1:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="195" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="196"/>
+      <c r="C15" s="209" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="206" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="46"/>
@@ -7098,43 +6984,43 @@
         <v>6</v>
       </c>
       <c r="J15" s="54"/>
-      <c r="K15" s="145"/>
-      <c r="L15" s="145"/>
-      <c r="M15" s="146"/>
-      <c r="N15" s="147">
+      <c r="K15" s="142"/>
+      <c r="L15" s="142"/>
+      <c r="M15" s="143"/>
+      <c r="N15" s="144">
         <v>1029271555.715</v>
       </c>
-      <c r="O15" s="134"/>
+      <c r="O15" s="131"/>
       <c r="P15" s="37"/>
       <c r="Q15" s="35"/>
       <c r="R15" s="10"/>
       <c r="V15" s="13"/>
     </row>
-    <row r="16" spans="1:22" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A16" s="211"/>
-      <c r="B16" s="212"/>
-      <c r="C16" s="304"/>
-      <c r="D16" s="302"/>
+    <row r="16" spans="1:22" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="197"/>
+      <c r="B16" s="198"/>
+      <c r="C16" s="210"/>
+      <c r="D16" s="207"/>
       <c r="E16" s="46"/>
       <c r="F16" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="148"/>
-      <c r="H16" s="148"/>
-      <c r="I16" s="149"/>
+        <v>74</v>
+      </c>
+      <c r="G16" s="145"/>
+      <c r="H16" s="145"/>
+      <c r="I16" s="146"/>
       <c r="J16" s="54"/>
-      <c r="K16" s="228" t="s">
+      <c r="K16" s="216" t="s">
         <v>49</v>
       </c>
-      <c r="L16" s="229"/>
-      <c r="M16" s="150">
+      <c r="L16" s="217"/>
+      <c r="M16" s="147">
         <f>M13+M14</f>
         <v>0</v>
       </c>
-      <c r="N16" s="151" t="s">
+      <c r="N16" s="148" t="s">
         <v>45</v>
       </c>
-      <c r="O16" s="134" t="s">
+      <c r="O16" s="131" t="s">
         <v>38</v>
       </c>
       <c r="P16" s="37"/>
@@ -7142,381 +7028,381 @@
       <c r="R16" s="10"/>
       <c r="V16" s="17"/>
     </row>
-    <row r="17" spans="1:21" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A17" s="105" t="s">
+    <row r="17" spans="1:21" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="152"/>
-      <c r="D17" s="153">
+      <c r="C17" s="149"/>
+      <c r="D17" s="150">
         <f>F4+F5-C17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="154"/>
+      <c r="E17" s="151"/>
       <c r="F17" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="148"/>
-      <c r="H17" s="148"/>
-      <c r="I17" s="149"/>
+        <v>75</v>
+      </c>
+      <c r="G17" s="145"/>
+      <c r="H17" s="145"/>
+      <c r="I17" s="146"/>
       <c r="J17" s="54"/>
-      <c r="K17" s="262" t="s">
+      <c r="K17" s="180" t="s">
         <v>50</v>
       </c>
-      <c r="L17" s="263"/>
-      <c r="M17" s="155">
+      <c r="L17" s="181"/>
+      <c r="M17" s="152">
         <f>(F13+L14)*1%</f>
         <v>0</v>
       </c>
-      <c r="N17" s="156"/>
-      <c r="O17" s="157">
+      <c r="N17" s="153"/>
+      <c r="O17" s="154">
         <v>0.01</v>
       </c>
       <c r="P17" s="37"/>
       <c r="Q17" s="35"/>
       <c r="R17" s="10"/>
     </row>
-    <row r="18" spans="1:21" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A18" s="219" t="s">
+    <row r="18" spans="1:21" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="190" t="s">
+      <c r="B18" s="199" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="152"/>
-      <c r="D18" s="153">
+      <c r="C18" s="149"/>
+      <c r="D18" s="150">
         <f>F6-C18</f>
         <v>0</v>
       </c>
-      <c r="E18" s="158" t="s">
+      <c r="E18" s="155" t="s">
         <v>45</v>
       </c>
       <c r="F18" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="148"/>
-      <c r="H18" s="148"/>
-      <c r="I18" s="149"/>
+        <v>77</v>
+      </c>
+      <c r="G18" s="145"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="146"/>
       <c r="J18" s="54"/>
-      <c r="K18" s="262" t="s">
+      <c r="K18" s="180" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="263"/>
-      <c r="M18" s="155">
+      <c r="L18" s="181"/>
+      <c r="M18" s="152">
         <f>F11</f>
         <v>0</v>
       </c>
-      <c r="N18" s="145"/>
-      <c r="O18" s="159"/>
+      <c r="N18" s="142"/>
+      <c r="O18" s="156"/>
       <c r="P18" s="37"/>
       <c r="Q18" s="35"/>
       <c r="R18" s="10"/>
     </row>
-    <row r="19" spans="1:21" ht="21.9" customHeight="1">
-      <c r="A19" s="219"/>
-      <c r="B19" s="190"/>
-      <c r="C19" s="152"/>
-      <c r="D19" s="153">
+    <row r="19" spans="1:21" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="208"/>
+      <c r="B19" s="199"/>
+      <c r="C19" s="149"/>
+      <c r="D19" s="150">
         <f t="shared" ref="D19:D23" si="5">F7-C19</f>
         <v>0</v>
       </c>
-      <c r="E19" s="158"/>
+      <c r="E19" s="155"/>
       <c r="F19" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="G19" s="160">
+      <c r="G19" s="157">
         <f>SUM(G16:G18)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="160">
+      <c r="H19" s="157">
         <f>SUM(H16:H18)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="160">
+      <c r="I19" s="157">
         <f>SUM(I16:I18)</f>
         <v>0</v>
       </c>
       <c r="J19" s="54"/>
-      <c r="K19" s="111"/>
-      <c r="L19" s="111"/>
-      <c r="M19" s="111"/>
-      <c r="N19" s="159"/>
-      <c r="O19" s="159"/>
+      <c r="K19" s="108"/>
+      <c r="L19" s="108"/>
+      <c r="M19" s="108"/>
+      <c r="N19" s="156"/>
+      <c r="O19" s="156"/>
       <c r="P19" s="37"/>
       <c r="Q19" s="35"/>
       <c r="R19" s="10"/>
     </row>
-    <row r="20" spans="1:21" ht="21.9" customHeight="1" thickBot="1">
-      <c r="A20" s="219"/>
-      <c r="B20" s="190"/>
-      <c r="C20" s="152"/>
-      <c r="D20" s="153">
+    <row r="20" spans="1:21" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="208"/>
+      <c r="B20" s="199"/>
+      <c r="C20" s="149"/>
+      <c r="D20" s="150">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E20" s="158"/>
+      <c r="E20" s="155"/>
       <c r="F20" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="298">
+      <c r="G20" s="186">
         <f>SUM(G19:I19)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="299"/>
-      <c r="I20" s="300"/>
+      <c r="H20" s="187"/>
+      <c r="I20" s="188"/>
       <c r="J20" s="54"/>
-      <c r="K20" s="111"/>
-      <c r="L20" s="111"/>
-      <c r="M20" s="111"/>
-      <c r="N20" s="159"/>
-      <c r="O20" s="161"/>
+      <c r="K20" s="108"/>
+      <c r="L20" s="108"/>
+      <c r="M20" s="108"/>
+      <c r="N20" s="156"/>
+      <c r="O20" s="158"/>
       <c r="P20" s="87"/>
       <c r="Q20" s="35"/>
       <c r="R20" s="10"/>
     </row>
-    <row r="21" spans="1:21" ht="29.4" customHeight="1" thickBot="1">
-      <c r="A21" s="105" t="s">
+    <row r="21" spans="1:21" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="152"/>
-      <c r="D21" s="153">
+      <c r="C21" s="149"/>
+      <c r="D21" s="150">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E21" s="162" t="s">
+      <c r="E21" s="159" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="159"/>
-      <c r="G21" s="111"/>
-      <c r="H21" s="163"/>
-      <c r="I21" s="164">
-        <v>0</v>
-      </c>
-      <c r="J21" s="163"/>
-      <c r="K21" s="163"/>
-      <c r="L21" s="111"/>
-      <c r="M21" s="111"/>
-      <c r="N21" s="165"/>
-      <c r="O21" s="166"/>
+      <c r="F21" s="156"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="160"/>
+      <c r="I21" s="161">
+        <v>0</v>
+      </c>
+      <c r="J21" s="160"/>
+      <c r="K21" s="160"/>
+      <c r="L21" s="108"/>
+      <c r="M21" s="108"/>
+      <c r="N21" s="162"/>
+      <c r="O21" s="163"/>
       <c r="P21" s="83"/>
       <c r="Q21" s="35"/>
       <c r="R21" s="10"/>
     </row>
-    <row r="22" spans="1:21" ht="19.5" customHeight="1" thickTop="1">
-      <c r="A22" s="105" t="s">
+    <row r="22" spans="1:21" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="167"/>
-      <c r="D22" s="153">
+      <c r="C22" s="164"/>
+      <c r="D22" s="150">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E22" s="154"/>
-      <c r="F22" s="191" t="s">
+      <c r="E22" s="151"/>
+      <c r="F22" s="266" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="266" t="s">
+      <c r="G22" s="182" t="s">
         <v>33</v>
       </c>
-      <c r="H22" s="267"/>
+      <c r="H22" s="183"/>
       <c r="I22" s="78"/>
       <c r="J22" s="79"/>
-      <c r="K22" s="260" t="s">
+      <c r="K22" s="193" t="s">
         <v>32</v>
       </c>
-      <c r="L22" s="261"/>
-      <c r="M22" s="268" t="s">
+      <c r="L22" s="194"/>
+      <c r="M22" s="184" t="s">
         <v>64</v>
       </c>
-      <c r="N22" s="165"/>
-      <c r="O22" s="265"/>
-      <c r="P22" s="264"/>
+      <c r="N22" s="162"/>
+      <c r="O22" s="179"/>
+      <c r="P22" s="178"/>
       <c r="Q22" s="35"/>
       <c r="R22" s="35"/>
     </row>
-    <row r="23" spans="1:21" ht="38.4" customHeight="1">
-      <c r="A23" s="105" t="s">
+    <row r="23" spans="1:21" ht="38.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="103" t="s">
+      <c r="B23" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="152"/>
-      <c r="D23" s="153">
+      <c r="C23" s="149"/>
+      <c r="D23" s="150">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E23" s="154"/>
-      <c r="F23" s="192"/>
-      <c r="G23" s="100" t="s">
+      <c r="E23" s="151"/>
+      <c r="F23" s="267"/>
+      <c r="G23" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="168">
+      <c r="H23" s="165">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I23" s="101"/>
-      <c r="J23" s="106"/>
-      <c r="K23" s="102" t="s">
+      <c r="I23" s="98"/>
+      <c r="J23" s="103"/>
+      <c r="K23" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="L23" s="169">
+      <c r="L23" s="166">
         <v>0.01</v>
       </c>
-      <c r="M23" s="269"/>
-      <c r="N23" s="165"/>
-      <c r="O23" s="265"/>
-      <c r="P23" s="264"/>
+      <c r="M23" s="185"/>
+      <c r="N23" s="162"/>
+      <c r="O23" s="179"/>
+      <c r="P23" s="178"/>
       <c r="Q23" s="22"/>
       <c r="S23" s="37"/>
       <c r="U23" s="4"/>
     </row>
-    <row r="24" spans="1:21" ht="27.65" customHeight="1" thickBot="1">
-      <c r="A24" s="203" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="204"/>
-      <c r="C24" s="152"/>
-      <c r="D24" s="153">
+    <row r="24" spans="1:21" ht="27.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="204" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="205"/>
+      <c r="C24" s="149"/>
+      <c r="D24" s="150">
         <f>F12-C24</f>
         <v>0</v>
       </c>
-      <c r="E24" s="154"/>
-      <c r="F24" s="192"/>
-      <c r="G24" s="194" t="s">
+      <c r="E24" s="151"/>
+      <c r="F24" s="267"/>
+      <c r="G24" s="269" t="s">
         <v>48</v>
       </c>
-      <c r="H24" s="255" t="s">
+      <c r="H24" s="273" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="273" t="s">
+      <c r="I24" s="285" t="s">
         <v>55</v>
       </c>
-      <c r="J24" s="274"/>
-      <c r="K24" s="281" t="s">
+      <c r="J24" s="286"/>
+      <c r="K24" s="293" t="s">
         <v>52</v>
       </c>
-      <c r="L24" s="252" t="s">
+      <c r="L24" s="244" t="s">
         <v>53</v>
       </c>
-      <c r="M24" s="223">
+      <c r="M24" s="211">
         <f>G28+L28+(L14*1%)</f>
         <v>0</v>
       </c>
-      <c r="N24" s="165"/>
-      <c r="O24" s="170"/>
+      <c r="N24" s="162"/>
+      <c r="O24" s="167"/>
       <c r="P24" s="88"/>
       <c r="Q24" s="4"/>
       <c r="S24" s="35"/>
     </row>
-    <row r="25" spans="1:21" ht="20.25" customHeight="1">
-      <c r="A25" s="289" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="290"/>
-      <c r="C25" s="270">
+    <row r="25" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="296" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="297"/>
+      <c r="C25" s="282">
         <f>SUM(C17:C24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="230">
+      <c r="D25" s="218">
         <f>SUM(D17:D24)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="154"/>
-      <c r="F25" s="192"/>
-      <c r="G25" s="195"/>
-      <c r="H25" s="256"/>
-      <c r="I25" s="275"/>
-      <c r="J25" s="276"/>
-      <c r="K25" s="282"/>
-      <c r="L25" s="253"/>
-      <c r="M25" s="224"/>
-      <c r="N25" s="165"/>
-      <c r="O25" s="171"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="267"/>
+      <c r="G25" s="270"/>
+      <c r="H25" s="274"/>
+      <c r="I25" s="287"/>
+      <c r="J25" s="288"/>
+      <c r="K25" s="294"/>
+      <c r="L25" s="245"/>
+      <c r="M25" s="212"/>
+      <c r="N25" s="162"/>
+      <c r="O25" s="168"/>
       <c r="P25" s="89"/>
       <c r="Q25" s="4"/>
       <c r="S25" s="35"/>
     </row>
-    <row r="26" spans="1:21" ht="20.25" customHeight="1">
-      <c r="A26" s="291"/>
-      <c r="B26" s="292"/>
-      <c r="C26" s="271"/>
-      <c r="D26" s="231"/>
-      <c r="E26" s="154"/>
-      <c r="F26" s="193"/>
-      <c r="G26" s="196"/>
-      <c r="H26" s="257"/>
-      <c r="I26" s="277"/>
-      <c r="J26" s="278"/>
-      <c r="K26" s="283"/>
-      <c r="L26" s="254"/>
-      <c r="M26" s="224"/>
-      <c r="N26" s="159"/>
-      <c r="O26" s="172"/>
+    <row r="26" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="298"/>
+      <c r="B26" s="299"/>
+      <c r="C26" s="283"/>
+      <c r="D26" s="219"/>
+      <c r="E26" s="151"/>
+      <c r="F26" s="268"/>
+      <c r="G26" s="271"/>
+      <c r="H26" s="275"/>
+      <c r="I26" s="289"/>
+      <c r="J26" s="290"/>
+      <c r="K26" s="295"/>
+      <c r="L26" s="246"/>
+      <c r="M26" s="212"/>
+      <c r="N26" s="156"/>
+      <c r="O26" s="169"/>
       <c r="P26" s="90"/>
       <c r="Q26" s="81"/>
       <c r="S26" s="35"/>
     </row>
-    <row r="27" spans="1:21" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A27" s="293"/>
-      <c r="B27" s="294"/>
-      <c r="C27" s="272"/>
-      <c r="D27" s="232"/>
-      <c r="E27" s="154"/>
+    <row r="27" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="300"/>
+      <c r="B27" s="301"/>
+      <c r="C27" s="284"/>
+      <c r="D27" s="220"/>
+      <c r="E27" s="151"/>
       <c r="F27" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="173"/>
-      <c r="H27" s="174">
-        <v>0</v>
-      </c>
-      <c r="I27" s="205"/>
-      <c r="J27" s="206"/>
-      <c r="K27" s="175"/>
-      <c r="L27" s="176"/>
-      <c r="M27" s="224"/>
-      <c r="N27" s="159"/>
-      <c r="O27" s="177"/>
+      <c r="G27" s="170"/>
+      <c r="H27" s="171">
+        <v>0</v>
+      </c>
+      <c r="I27" s="280"/>
+      <c r="J27" s="281"/>
+      <c r="K27" s="172"/>
+      <c r="L27" s="173"/>
+      <c r="M27" s="212"/>
+      <c r="N27" s="156"/>
+      <c r="O27" s="174"/>
       <c r="P27" s="90"/>
       <c r="Q27" s="81"/>
       <c r="R27" s="35"/>
     </row>
-    <row r="28" spans="1:21" ht="24.75" customHeight="1" thickTop="1" thickBot="1">
+    <row r="28" spans="1:21" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="46"/>
-      <c r="B28" s="178"/>
-      <c r="C28" s="154"/>
-      <c r="D28" s="154"/>
-      <c r="E28" s="154"/>
+      <c r="B28" s="175"/>
+      <c r="C28" s="151"/>
+      <c r="D28" s="151"/>
+      <c r="E28" s="151"/>
       <c r="F28" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="279">
+      <c r="G28" s="291">
         <f>(G27+H27)*H23</f>
         <v>0</v>
       </c>
-      <c r="H28" s="280"/>
-      <c r="I28" s="226"/>
-      <c r="J28" s="227"/>
-      <c r="K28" s="179"/>
-      <c r="L28" s="180">
+      <c r="H28" s="292"/>
+      <c r="I28" s="214"/>
+      <c r="J28" s="215"/>
+      <c r="K28" s="176"/>
+      <c r="L28" s="177">
         <f>(I27+K27+L27)*L23</f>
         <v>0</v>
       </c>
-      <c r="M28" s="225"/>
-      <c r="N28" s="159"/>
+      <c r="M28" s="213"/>
+      <c r="N28" s="156"/>
       <c r="O28" s="92"/>
       <c r="P28" s="92"/>
       <c r="Q28" s="81"/>
       <c r="R28" s="35"/>
     </row>
-    <row r="29" spans="1:21" ht="12" customHeight="1" thickTop="1">
+    <row r="29" spans="1:21" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A29" s="46"/>
       <c r="B29" s="47"/>
       <c r="C29" s="25"/>
@@ -7536,15 +7422,15 @@
       <c r="Q29" s="82"/>
       <c r="R29" s="35"/>
     </row>
-    <row r="30" spans="1:21" ht="34.5" customHeight="1">
+    <row r="30" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="46"/>
-      <c r="B30" s="189" t="s">
+      <c r="B30" s="279" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="189"/>
-      <c r="D30" s="189"/>
-      <c r="E30" s="189"/>
-      <c r="F30" s="189"/>
+      <c r="C30" s="279"/>
+      <c r="D30" s="279"/>
+      <c r="E30" s="279"/>
+      <c r="F30" s="279"/>
       <c r="G30" s="48"/>
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
@@ -7558,15 +7444,15 @@
       <c r="Q30" s="82"/>
       <c r="R30" s="35"/>
     </row>
-    <row r="31" spans="1:21" s="40" customFormat="1" ht="160.5" customHeight="1">
+    <row r="31" spans="1:21" s="40" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="189"/>
-      <c r="C31" s="189"/>
-      <c r="D31" s="189"/>
-      <c r="E31" s="189"/>
-      <c r="F31" s="189"/>
+      <c r="B31" s="279"/>
+      <c r="C31" s="279"/>
+      <c r="D31" s="279"/>
+      <c r="E31" s="279"/>
+      <c r="F31" s="279"/>
       <c r="G31" s="68" t="s">
         <v>41</v>
       </c>
@@ -7585,7 +7471,7 @@
       <c r="Q31" s="45"/>
       <c r="R31" s="45"/>
     </row>
-    <row r="32" spans="1:21" ht="31.5" hidden="1" customHeight="1">
+    <row r="32" spans="1:21" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>19886411</v>
       </c>
@@ -7611,7 +7497,7 @@
       <c r="M32" s="3"/>
       <c r="N32" s="21"/>
     </row>
-    <row r="33" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+    <row r="33" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="8" t="s">
         <v>14</v>
       </c>
@@ -7641,7 +7527,7 @@
       <c r="M33" s="44"/>
       <c r="N33" s="4"/>
     </row>
-    <row r="34" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+    <row r="34" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="14" t="e">
         <v>#REF!</v>
       </c>
@@ -7670,7 +7556,7 @@
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
     </row>
-    <row r="35" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+    <row r="35" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="5" t="e">
         <v>#REF!</v>
       </c>
@@ -7693,7 +7579,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:14" ht="31.5" hidden="1" customHeight="1">
+    <row r="36" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C36" s="13" t="e">
         <v>#REF!</v>
       </c>
@@ -7703,93 +7589,86 @@
       <c r="G36" s="23"/>
       <c r="H36" s="24"/>
     </row>
-    <row r="37" spans="1:14" ht="31.5" customHeight="1">
+    <row r="37" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="10" t="s">
         <v>4</v>
       </c>
       <c r="G37" s="11"/>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:14" ht="31.5" customHeight="1">
+    <row r="38" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C38" s="34"/>
     </row>
-    <row r="41" spans="1:14" ht="31.5" customHeight="1">
+    <row r="41" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="64"/>
     </row>
-    <row r="43" spans="1:14" ht="31.5" customHeight="1">
+    <row r="43" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="31.5" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" t="s">
         <v>81</v>
       </c>
-      <c r="B44" t="s">
+    </row>
+    <row r="45" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="96" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A45" s="98" t="s">
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="96" t="s">
         <v>83</v>
       </c>
-      <c r="B45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A46" s="98" t="s">
+      <c r="B46" t="s">
         <v>84</v>
       </c>
-      <c r="B46" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" ht="31.5" customHeight="1">
+    </row>
+    <row r="47" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" ht="31.5" customHeight="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:H3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="B30:F31"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="I24:J26"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="M24:M28"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="A25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="G20:I20"/>
     <mergeCell ref="A15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:D16"/>
@@ -7806,31 +7685,38 @@
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="I14:K14"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="I24:J26"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="M24:M28"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="A25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="B30:F31"/>
-    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>